<commit_message>
baseline code with semantic chuncker
</commit_message>
<xml_diff>
--- a/context.xlsx
+++ b/context.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10402"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masang/Desktop/aiffel/mini-aiffelton/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9995E3C-78B5-0D46-86F8-EE6A219CC95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
   <si>
     <t>Query</t>
   </si>
@@ -61,27 +55,24 @@
     <t>2020년 사업평가 점수가 떨어진 이유는 뭘까?</t>
   </si>
   <si>
-    <t>▷ 고객만족도 제고를 위한 기초조사실시의 필요성 부각
+    <t>연구배경 및 목적
+1. 연구의 배경민원행정서비스에 대한 만족도 조사는 한국행정연구원에서 1996년 조사모델과 방법을 개발한 이후 현재까지 지속적으로 수행하고 있는 중앙정부 및 지방정부의 과제이다. 횡성군 민원행정서비스 만족도조사는 횡성군 종합민원실에서 제공하는 민원행정서비스를 이용한 지역주민과 이용객을 대상으로 하여 행정서비스의 전달체계와 그 서비스 과정에서의 공무원들의 행태와 민원제도 등에 대해 체감하는 만족도를 조사하고자 실시되었다. 특히 상반기조사결과를 비교 대상으로 하여 하반기 고객 만족도의 수준을 평가하고 발전지향적인 고객중심의 행정서비스 체제를 구축하는데 있어 자료로 활용함으로써 횡성군이 제공하는 민원행정서비스의 질적 향상에 기여하고자 한다. ▷ 친절하고 쾌적한 민원실
+▷ 고객중심의 초일류 민원 행정기관으로서의 위상정립
+▷ 이용고객에 대한 과학적 분석을 토대로 장기발전전략 수립
+▷ 고객만족도 제고를 위한 기초조사실시의 필요성 부각
 ▷ 눈높이 민원행정의 실현
 2. 연구의 목적
-횡성군 종합민원실에서 제공하는 행정서비스의 고객인 이용자들로 하여금 민원행정서비스의 전달체계와 그 서비스 과정에서 공무원들의 행태와 민원 제도, 시설 등에 대하여 체감정도를 조사를 목적으로 하고 있다. 
-횡성군 민원행정 서비스 고객만족도 조사는 구체적으로 다음과 같은 의의를 내포하고 있다. 
-▷ 고객중심의 초일류 민원행정서비스의 실현
+횡성군 종합민원실에서 제공하는 행정서비스의 고객인 이용자들로 하여금 민원행정서비스의 전달체계와 그 서비스 과정에서 공무원들의 행태와 민원 제도, 시설 등에 대하여 체감정도를 조사를 목적으로 하고 있다. 횡성군 민원행정 서비스 고객만족도 조사는 구체적으로 다음과 같은 의의를 내포하고 있다. ▷ 고객중심의 초일류 민원행정서비스의 실현
 ▷ 고객만족도 제고 및 고객감동 지향
 ▷ 불합리한 제도개선과 발전방향 제시
 ▷ 맞춤형 민원행정 서비스 실현
 ▷ 전자민원 행정구현을 위한 기초조사
 ▷ 행정업무 분야별 만족도 제고
-▷ 행정서비스의 취약점과 개선방향을 도출</t>
-  </si>
-  <si>
-    <t>▷ 행정업무 분야별 만족도 제고
 ▷ 행정서비스의 취약점과 개선방향을 도출
-▷ 과거의 고객만족도 결과와 비교하여 고객만족도 수준의 변화정도를 분석고객만족도 조사는 궁극적으로 평가대상이 되는 종합민원실로 하여금 고객중심의 행정서비스를 구현하며, 행정서비스의 질을 향상시킴으로써 횡성군의 경쟁력 제고를 궁극적인 목표로 하고 있다고 할 수 있다. 
-II. 연구범위 및 방법
-1. 연구범위
-▷ 시간적 범위
-- 2006. 10. 27 ~ 2006. 11. 30(35일)
+▷ 과거의 고객만족도 결과와 비교하여 고객만족도 수준의 변화정도를 분석고객만족도 조사는 궁극적으로 평가대상이 되는 종합민원실로 하여금 고객중심의 행정서비스를 구현하며, 행정서비스의 질을 향상시킴으로써 횡성군의 경쟁력 제고를 궁극적인 목표로 하고 있다고 할 수 있다. II.</t>
+  </si>
+  <si>
+    <t>11. 30(35일)
 ▷ 공간적 범위
 - 횡성군 종합민원실
 ▷ 내용적 범위
@@ -92,60 +83,196 @@
 - 종합평가 및 발전방안
 2. 연구방법
 ▷ 문헌연구 및 자료분석(literature study &amp; data analysis)
-▷ 설문조사</t>
-  </si>
-  <si>
-    <t>제1장 연구개요
-I. 연구배경 및 목적
-1. 연구의 배경민원행정서비스에 대한 만족도 조사는 한국행정연구원에서 1996년 조사모델과 방법을 개발한 이후 현재까지 지속적으로 수행하고 있는 중앙정부 및 지방정부의 과제이다. 
-횡성군 민원행정서비스 만족도조사는 횡성군 종합민원실에서 제공하는 민원행정서비스를 이용한 지역주민과 이용객을 대상으로 하여 행정서비스의 전달체계와 그 서비스 과정에서의 공무원들의 행태와 민원제도 등에 대해 체감하는 만족도를 조사하고자 실시되었다. 
-특히 상반기조사결과를 비교 대상으로 하여 하반기 고객 만족도의 수준을 평가하고 발전지향적인 고객중심의 행정서비스 체제를 구축하는데 있어 자료로 활용함으로써 횡성군이 제공하는 민원행정서비스의 질적 향상에 기여하고자 한다. 
-▷ 친절하고 쾌적한 민원실
-▷ 고객중심의 초일류 민원 행정기관으로서의 위상정립
-▷ 이용고객에 대한 과학적 분석을 토대로 장기발전전략 수립
-▷ 고객만족도 제고를 위한 기초조사실시의 필요성 부각</t>
-  </si>
-  <si>
-    <t>3. 설문지 구성
-민원행정서비스에 대한 이용고객의 만족도를 평가하기 위한 설문문항은 중앙행정기관 대국민 행정서비스에 대한 공공고객 만족도 조사에 이용된 설문과 광역지방자치단체의 만족도 조사에 이용된 항목중에서 추출하였으며 크게 민원시설, 서비스, 민원처리, 인구통계적인 요소로 구성하였다. 
-세부설문 항목은 민원행정 시설과 관련한 5개 문항과 민원안내 서비스 및 친절도와 관련한 5개 문항, 민원처리와 관련한 7개 문항, 인구통계적인 항목 4개, 기타 1개로 총 22개 항목으로 구성하였다. 
-상반기 조사에 활용된 설문항목에서 분야별 종합만족도에 대한 설문항목은 제외하였으며, 업무담당자와 민원처리부서의 업무처리방법에 대한 설문이 추가되었다. 
-설문문항은&lt;|start|&gt;#@이름1#&lt;|end|&gt;에 의해 개발된 총화평정법에 의한 척도구성법인 Likert 5 level scale로 등간척도 문항을 구성하였다. 
-4. 분석방법</t>
-  </si>
-  <si>
-    <t>○ 조사대상 업종 및 대상 확대
-- 조사대상 업종의 확대: 저임금 근로자가 집중된 산업에서 저임금 근로자가 집중된 사업체를 선정하여 해당 산업 및 사업체의 저임금 근로자와 사용자에게 설문을 진행하는 현행 방식으로, 조사 결과에서의 저임금 근로자의 특성은 경제 전체에서의 최저임금 수급자와 차이가 있음. 본 조사의 결과를 전국 단위로 적용되는 최저임금의 심의자료로 활용하기 위해서는 전체 산업별, 사업체 규모별, 사업체 수 및 피고용인의 수를 고려하여 표본설계후, 저임금 근로자가 있는 사업장에 대해 진행하되, 저임금 근로자가 없는 사업장의경우 없다는 것을 표본에 대한 기초통계에 제시
-- ‘영세·소규모 사업장에 대한 영향 분석’ 혹은 ‘전체 사업장에 대한 영향 분석’으로 목적을 구분하고, 그에 맞는 모집단의 범위 설정 필요</t>
-  </si>
-  <si>
-    <t>- 과연 임금분포 상 어떤 범위의 저임금 근로자들의 임금이 상대적으로 상승하여 임금격차 해소에 일조하는지, 또 임금분포 상 어떤 범위의 저임금 근로자들이 고용 측면에서 영향 하에 놓이게 되는지를 살펴보면 실태조사의 조사대상 근로자 선정기준을 명확히 하는 데 큰 시사점을 얻을 수 있음
-○ 본 장에서는 최저임금(인상)이 임금불평등(또는 격차)과 고용에 미치는영향을 임금분포를 기준으로 분석한 연구들을 소개함
-○ 이상의 분석결과를 종합하면 최저임금 인상은 최저임금 상위 계층의임금수준도 높이고, 임금분포도 압축시킴
-- 최저임금 인상은 직접적으로 영향을 받는(spike effect)최저임금 계층의 근로자 뿐만 아니라 간접적으로 영향을 받는(spillover effect)직상위 나아가 상위계층 근로자의임금수준에도 명백히 양(+)의 영향을 미치고 있음
-- 또한 최저임금 인상은 임금분위수배율의 변화에서도 관찰되는데, 최저임금의 인상은 임금분포를 압축시키고 있음
-○ 분석 결과</t>
-  </si>
-  <si>
-    <t>본 연구에서 도출된 결과 및 제언들은 다음과 같다. 
-첫째, 「최저임금 적용효과에 관한 실태조사」는 조사대상 사업체와 근로자에 대해 ‘최저임금액의 1.5배 이하를 받는 저임금 근로자와 이들을 고용하는 사업주’로 설정하고 있는데, 향후 조사에서는 조사대상 근로자에 대한 보다 명확하고 합리적인 기준 설정이 필요한 것으로 판단된다. 그동안 최저임금이 지속적으로 상승하면서 최저임금의 1.5배가 최근에는 거의 중위임금 수준까지 다다른 상황에서 현행 조사대상 근로자 선정 방식을 유지하는 것에 대한 검토가 필요하다는 것이다. 본 연구에서는 최저임금(인상)이 임금분포 상에서의 근로자들의 임금과 고용에 미치는 영향에 대한 실증 연구의 결과를 토대로 조사대상 근로자를, 1)현행대로 최저임금의 1.5배 이하 근로자로 설정하는 방안, 2)중위임금 이하 근로자를 조사대상으로 삼는 방안, 3)중위임금의 2/3 이하 근로자를 조사대상으로 삼는 방안 등 세 가지 안을 제시하였다.</t>
-  </si>
-  <si>
-    <t>현행 방식을 유지하는 방안은 통계작성의 일관성을 유지할 수 있는 장점이 있는 반면에 최저임금이 지속적으로 상승할 경위 최저임금의 1.5배가 중위 임금을 넘어설 가능성이 있어 조사대상 ‘저임금’ 근로자에 대한 논란이 지속될 수 있다. 중위임금 이하 근로자를 조사대상 근로자 선정기준으로 삼는 방안은 중위임금이 임금분포 상에서의 지표이기 때문에 쉽게 이해할 수 있고 최저임금의 변동과 상관 없이 일정 수준(전체 근로자의 절반)의 근로자들을 조사대상으로 삼기 때문에 조사대상 모집단의 일관성 유지 측면에서 이점을 가지는 방안이다. 중위임금의 2/3 이하 근로자를 조사 대상으로 삼는 방안은 중위임금의 2/3 이하가 국제적으로 통용되는 통상적인 저임금 근로자의 정의에 부합한다는 점에서 장점이 있는 반면, 현행 방식 보다 포괄되는 조사대상이 협소하게 됨에 따라 조사대상 사업체 및 근로자 추출에 있어 현실적이 어려움이 클 것으로 예상된다. 이들 각 방안의 장단점 들을 고려하여 현실에 맞는 조사대상</t>
-  </si>
-  <si>
-    <t>〇 우선적으로 고려할 사항을 질문하는 항목은 복수응답 개수를 제한하여순위 질문으로 변경하는 방안 검토 필요함
-〇 최저임금과 직접 관련된 내용으로 보이지 않은 항목 검토 필요함
-〇 문항 배치 검토 필요
-〇 가구 전체 소득 및 지출금액으로 최대범위(500만원 이상)가 다소 적은것으로 보이므로 검토 필요함
-〇 사업장의 고지 여부를 근로자에게 질문하는 것이 적절한지 검토 필요함
-5. 조사체계
-○ 조사의 정확성과 효율성 제고를 위해 그동안 각 지방관서별로 이루어졌던조사계획 수립, 조사원 채용 및 교육 등을 조사 전문기관에서 일괄적으로수행
-- 근로감독관은 조사 불응 사업체에 대한 조사 지원 업무를 담당하고 조사기관은 조사대상에 대한 현장조사를 강화하여 응답률 제고
-○ 최저임금 근로자가 상대적으로 많이 분포하는 기업규모 군에 대해 선정가능한 근로자 수를 증가시킬 수 있도록 조사의 우선순위 기준 명확화</t>
-  </si>
-  <si>
-    <t>4. 조사표 구성
+▷ 설문조사
+- 조사요원 : 2명의 설문조사원(투입전 사전교육 수료)
+- 조사기간: 2006년 11월 2일 ~ 2006년 11월 15일(10일간)
+- 조사장소: 횡성군 종합민원실
+- 조사방법: 1:1 면접식 설문조사 및 자기기입식 조사실시
+제2장 조사분석
+I. 조사설계
+1. 조사대상
+▷ 2006년 11월 2일부터 11월 15일까지 13일 중 공휴일과 휴일을 제외한 10일을 선정하여 횡성군 종합민원실의 민원행정서비스를 이용한 민원인 중 인 524명을 대상으로 함. (단, 민원실을 이용한 개인만을 그 대상으로 하였고, 민원대행업무를 보는 법무사 등의 기관이나 단체는 제외하였음. )
+▷ 모집단 및 표본추출방법
+- 1단계: 전체 민원행정서비스 이용자를 대상으로 하였음. - 2단계: 민원분야별로 균형 있는 결과 도출을 위하여 가능한 범위내에서 샘플을 통제하고자 하였음. (6개 민원업무별)
+- 3단계: 최초 500명에서 524명으로 조사대상이 증가한 이유는 상대적으로 낮은 샘플수를 기록한 업무분야에 대한 조사를 추가적으로 실시하고자 하였으나 민원인이 적은 관계로 소기의 목적은 달성하지 못하였음. ※ 2006년 상반기 고객만족도 조사에서 민원인들의 지역별 분배를 통하여 결과를 도출한바, 유의한 수준으로 분석되지 않아 하반기 조사에서는 지역별 안배는 배제하였음. 2. 조사기간 :
+▷ 2006년 11월 2일 ~ 11월 15일(10일간)
+▷ 조사도구: 구조화된 조사표(Structured Questionnaire)
+▷ 설문조사실시:
+- 설문조사는 조사대상자 524명에 대하여 횡성군 종합민원실내에서 실시하였으며, 설문에 참여한 대상자들에게는 소정의 설문기념품을 제공함. - 사전교육을 받은 2명의 조사원들이 1:1 면접식 조사방법과 자기기입식 방법으로 설문조사를 실시함. 3. 설문지 구성
+민원행정서비스에 대한 이용고객의 만족도를 평가하기 위한 설문문항은 중앙행정기관 대국민 행정서비스에 대한 공공고객 만족도 조사에 이용된 설문과 광역지방자치단체의 만족도 조사에 이용된 항목중에서 추출하였으며 크게 민원시설, 서비스, 민원처리, 인구통계적인 요소로 구성하였다. 세부설문 항목은 민원행정 시설과 관련한 5개 문항과 민원안내 서비스 및 친절도와 관련한 5개 문항, 민원처리와 관련한 7개 문항, 인구통계적인 항목 4개, 기타 1개로 총 22개 항목으로 구성하였다. 상반기 조사에 활용된 설문항목에서 분야별 종합만족도에 대한 설문항목은 제외하였으며, 업무담당자와 민원처리부서의 업무처리방법에 대한 설문이 추가되었다. 설문문항은&lt;|start|&gt;#@이름1#&lt;|end|&gt;에 의해 개발된 총화평정법에 의한 척도구성법인 Likert 5 level scale로 등간척도 문항을 구성하였다. 4. 분석방법
+수집된 자료에 대한 분석방법은 통계적 방법을 적용하였는데, 통계처리는 Data- Coding 과정을 거쳐 통계패키지인 SPSS for win 12.0을 활용하여 분석하였다. 수집된 자료의 분석을 위해 기술적 통계(descriptive statistics)는 모든 변수의 빈도분석표와 기술통계량을 제공받고자 평균(mean), 표준편차(std. )등을 적용하였다. 성별에 따른 차이검증을 위하여 T- test가 사용되었으며 연령별, 거주지별, 민원업무별 차이에 따른 만족도의 비교분석을 위하여 분산분석(ANOVA)을 실시하였다. 만족도 산정방식은 항목별로 5점 척도를 사용하였다. 매우만족은 1점, 매우불만족은 5점으로 측정하고 이것을 다시{(i-1)/4}×100을 통해 100점 척도로 환산하였다. II.</t>
+  </si>
+  <si>
+    <t>발전방안
+1. 만족도 평가와 비교분석을 통한 문제점 탐색
+▷ 2006년 상반기 조사결과에서 도출된 만족도 점수와 순위를 하반기 결과와 비교하여 연결한 결과 편의시설 항목이 가장 만족도가 높게 평가되었음. ▷ 각 차원에 대한 종합만족도는 세부항목간의 분석에 영향을 미칠수 있어 하반기 설문에서는 배제하였음. ▷ 민원인들이 가장 불편하게 느끼고 있는 것은 주차장시설로 나타났으며, 상·하반기 만족도 조사결과에서도 최하위를 기록하고 있어 개선이 필요함. ▷ 민원인이 민원실로 들어오면서 민원을 어떻게 신청하고 민원창구가 어디에 위치하고 있는 지에 대한 설명을 제공하는 항목에 대한 만족도는 상·하반기를 종합하여 10위로 나타남. ▷ 온라인을 통한 민원안내와 상담에 대한 만족도가 상대적으로 낮게 평가되고 있음. 계획적이고 체계적인 만족도 조사를 실시함으로써 고객
+▷ 지향적 민원행정 서비스 개선방법과 만족도를 제고시킬 수 있는 마인드 제고
+2. 수준별 관리내용 제안
+분석결과를 토대로 하여 긴급개선분야, 개선권장분야, 현상유지분야, 개선유지분야의 4개 영역으로 차원수준이나 항목으로 구분하여 중요도에 따른 관리 및 개선이 이루어 질 수 있도록 함. ▷ 2006년 상반기의 분석결과 긴급하게 개선되어야 할 분야로서 주차장 시설과 민원처리의 신속성에 대한 항목이 도출되었으나 2006년 하반기의 조사분석결과 시설부분에 있어 주차장과 안내서비스와 관련한 항목, 온라인을 이용한 상담 및 문의에 대한 항목에 대한 개선이 요구되고 있는 것으로 분석됨. ▷ 횡성군 종합민원실의 행정서비스에서 가장 우선적으로 개선되어야 할 사항은 민원인들이 이용하는 주차공간에 대한 개선이 시급히 이루어져야 함. (무료이용, 공간확대, 복층화 등)
+▷ 민원창구의 업무담당자가 자리를 비우게 될시 이를 보충할 수 있는 보조인력이 상시 대기할 수 있도록 하여 민원업무의 연속성이 확보되어야 함. ▷ 온라인을 이용한 민원상담과 문의 등에 능동적이고 적극적으로 서비스 할 수 있도록 하여야 함. (홈페이지의 접속용이성을 높이고 온라인으로 가능한 민원처리 안내 등이 우선적으로 선행되어야 함. )
+▷ 민원업무 담당자들을 대상으로 한 친절 및 예절교육을 주기적으로 실시하여 민원인들로 하여금 이웃과 같은 친근함을 느낄 수 있도록 하여야 함. ▷ 민원 처리절차에 대한 정보를 민원실내에서 쉽게 확인하고 이에 따라 민원을 신청하고 처리할 수 있도록 도우미(공무원, 공익근무요원 등 활용)를 창구에 배치하는 것도 만족도를 제고하는 좋은 대안이 될 수 있음. ▷ 현행 민원창구의 테이블의 높이를 대폭 낮출 경우(예- 은행의 상담 창구)민원인들이 보다 친근감을 느낄 수 있을 것이고, 민원업무 전반에 걸친 거부감이나 부담감이 현저히 저하되어 고객만족도가 대폭 향상될 것임(현재 직각형인 모양을 물결모양으로 구성하면 민원업무별로 자연스러운 구분이 될 수도 있음. )
+전자기록물 장기보존패키지 - 제2부: 디렉토리로 구조화된 방식(NEO3)
+1. 적용범위
+이 표준은 디지털객체에 대한 논리적 또는 물리적 캡슐화 규격을 규정하는 동시에 진본성, 무결성, 이용가능성을 유지하기 위한 디지털기록물에 대한 장기보존패키지에 대한 기술규격을 기술하는 것으로, 「공공기록물 관리에 관한 법률」에 명시된 공공기관 및 기록물관리기관이 전자기록물을 장기간 보존해야 하는 경우 적용할 수 있다. 다만, 영구기록물관리기관, 동법 시행령 제3조 각 호에 해당하는 공공기관 등 전자기록물을 장기간 보존하는 기록물관리기관(이하'영구기록물관리기관 등'으로 칭함)은 소장 기록물의 특성, 기관의 환경 등에 따라 전자기록물의 장기보존패키지 방식을 달리 정할 수 있다. 비고 2
+이 표준에서 제시되는 장기보존패키지는 ISO 14721 OAIS(Open Archival Information System)참조모형에서 말하는 기록관에서 영구기록물관리기관으로 전자기록물을 이관하는 포맷(SIP, Submission Information Package), 이용자에게 전자기록물을 제공하는 포맷(DIP, Dissemination Information Package)등으로도 활용될 수 있다. 2. 적용근거
+이 표준의 구체적인 법적 근거는 다음과 같다. ㆍ 「공공기록물 관리에 관한 법률」제20조(전자기록물의 관리)
+ㆍ 「공공기록물 관리에 관한 법률」시행령 제36조(기록관 및 특수기록관의 전자기록물 보존)
+ㆍ 「공공기록물 관리에 관한 법률」시행령 제40조(기록관 및 특수기록관의 소관 기록물 이관)
+ㆍ 「공공기록물 관리에 관한 법률」시행령 제46조(영구기록물관리기관의 전자기록물 보존 및 관리)
+2.2 인용표준
+다음의 인용표준은 이 표준의 적용을 위해 필수적이다. 발행연도가 표기된 인용표준은 인용된 판만을 적용한다.</t>
+  </si>
+  <si>
+    <t>○ 여론주도층은 구청 관련 공무원 및 사회복지 기관 종사자를 중심으로 선정하였으며, 관련 공무원은 구청 주민생활과, 사회복지과, 가정복지과, 고용정책과, 보건소, 동사무소 사회복지전담공무원을, 그리고 실무자 집단은 사회복지 기관 종사자로 용산구 관내 복지기관 종사자를 조사 대상으로 함. 3）설문구성
+설문지는 용산구 관련 정책 자료와 기존의 지역사회 욕구조사 자료를 토대로 하여 개발하였으 며, 전문가 회의를 통한 설문지 검토 및 사전조사(pre- test)를 실시한 후 최종 확정함. 조사 내용은 크게 일반적 특성, 지역복지 환경 평가，복지수요 및 개선방안, 분야별 복지수요, 보건 및 의료서비스, 지역복지 참여 등의 영역으로 구성하여 각 영역에 해당하는 세부 사항들로 구 성함. 특히, 설문구성은 가족일반, 영유아복지, 여성복지, 아동복지, 청소년복지, 노인복지 등 다양한 분야의 욕구를 포함하였고, 각 대상별로 보다 세부적인 관련 욕구 및 개선사안, 향후 역점사업 등을 질문함. 여론주도층 및 실무자 조사에서는 현안 문제점, 정책개선사안, 향후 역점사업을 중심으로 설문을 구성하였음. 4）조사절차
+조사연구진이 보건복지부의 매뉴얼을 토대로 수정•보완하여 작성한 욕구조사표는 사회복지 실무진의 자문과 예비조사를 거쳐 최종 확정함. 이렇게 작성된 최종 조사표는 용산구 내 5개 권역 16개동에 배포하여 현장조사요원을 통한 설문조사가 실시되었음. 다문화가정은 조사대상자는 16개 주민센터에 배포되어 설문조사가 실시되었음. 1,306부롤 수집하여 유효데이터 1,288부를 분석하였음(유효율: 98.6%). 3.2 일반구민 욕구조사
+3.2.1 조사개요
+용산구에 거주하는 일반구민의 복지욕구를 분석하기 위해 본 조사에서는 용산구에 거주하고 있는 일반구민을 모집단으로 설정하고, 성별, 동별, 연령을 고려하여 160명을 비례층화 표본 추출하였다. 또한, 조사원이 조사대상의 기관(시설)또는 가정을 직접 방문하여 일대일 면접조사를 시실하였다. 설문 문항은 총 45문항으로서, 구체적 조사내용 항목은 지역복지 일반에 관한 용산구주민들의 의식조사, 거주 지역 서비스 및 현황에 대한 평가, 향후 사회복지 발전을 위한 우선순위, 사회복지시설 이용경험 및 만족도, 거주지 선택의 고려사항, 생활수준과 삶의 질, 사족생활상의 문제, 여가와 지역사회 활동, 자원봉사 및 불우이웃 후원 경험 및 향후 참여의 의향, 용산구가 실시하는 사회복지사업 및 보건사업에 대한 인지도와 만족도, 건강상태 등의 사항이 포함되어 있다. 분석방법으로는 전체적으로 빈도분석을 사용하였고, 만족도 등과 관련해서는 기술통계를 추가 이용하였으며, 필요에 따라 도표를 사용하였다.</t>
+  </si>
+  <si>
+    <t>3. Z3 종합분석
+용산구 일반주민의 복지욕구를 조사하기 위해, 동별 인구 비례를 감안하여 각 동별 표본 추출 사례 수를 정한 뒤에 전체 16개동으로부터 총 160가구의 주소를 무작위 추출하여 조사원들이 표본 추출된 가구들을 직접 방문 조사하는 지역비례 충화 표본(area stratified sampling)의 면접조사를 실시하였다. 첫째로, ‘보다 살기 좋은 사회’를 만들기 위하여 제도적 차원에서 힘써야 할 사항은 가중치 분석결과 ‘고용안정’29.7% _서居 및 물가안정* 26.9%, , • 신뢰회복 8.7%, , •복지시설 8.0% 순으로 나타났다.</t>
+  </si>
+  <si>
+    <t>조사대상 저임금 근로자의 포괄 범위
+○ 조사대상 저임금 근로자의 포괄 범위를 어떻게 설정하느냐에 대한 하나의 유일한 정답은 없음
+- 그 이유는 조사대상 저임금 근로자의 포괄 범위 설정을 위한 이론이나 특별한 방법이 정해져 있는 것도 아니고, 범위 설정에 대해서는 관련되어 있는 이해관계자 집단(stakeholder)마다 서로 다른 입장과 견해를 가지고 있기 때문임
+○ 합리적인 포괄 범위 설정을 위해서는 범위 설정의 기준 또는 원칙을 세우고, 실증적인 분석 결과들을 참고하여 방안들을 마련하고, 각 대안들의 장단점들을 종합적으로 고려한 후 조사의 목적에 부합하는 가장 현실적으로 선호되는 방안을 찾아내는 과정이 필요함
+1.1 조사대상 저임금 근로자 포괄 범위 설정의 네 가지 기준
+○ 객관성
+- 일반적으로 통용·수용될 수 있어야 하며, 국제적 비교가 가능하도록 설정되어야 함
+○ 일관성(시계열적 안정성)
+- 시기 간 비교가 가능하도록 일관되게 설정되어야 함
+○ 목적 부합성
+- 조사의 특수한 목적에 부합하도록 설정되어야 함
+- 누가 최저임금(인상)의 영향을 받는 집단인가?</t>
+  </si>
+  <si>
+    <t>최저임금 등 임금분포와 조사대상
+○ 최저임금과 비교되는 시급 임금분포와 최저임금의 중위임금에 대비한 상대적 수준 추이는'최저임금 적용효과에 관한 실태조사'의 조사대상 선정기준이 현재 시점에서도 적절한지 판단하는 데 유용한 역할을 할 수 있음
+- 최저임금과 비교되는 시급은 최저임금에 산입되는 개별 임금항목, 법정유급시간까지 포함한 근로시간 등에 대한 조사상의 제약으로, 최저임금위원회의 최저임금 심의에서 활용되는 공식자료에서는 다음과 같이 집계함
+- 경제활동인구 부가조사를 분석한 자료에서는 시급 = 월평균 임금총액 / 월 평소 근로시간(=주당 평소근로시간×(30.4/7)
+- 고용형태별 근로실태조사를 분석한 자료에서는 시급 = 월 통상임금 / 월 소정실 근로시간.</t>
+  </si>
+  <si>
+    <t>조사대상 업종 및 사업체 규모 범위 확대
+〇 현행 「최저임금 적용효과에 관한 실태조사」의 모집단은 저임금 근로자의고용 비중이 높은 업종(C, G, H, I, L, N, P, Q, R, S)의 상용근로자 300인 미만의 사업체로 국한하고 있음
+〇 이 조사의 모집단을 저임금 근로자를 고용하고 있는 사업체로 국한하는경우라도 현행 조사대상 업종과 사업체 규모를 전체 사업체로 확대할것인가의 문제는 추가로 검토해야 할 사항임. 원칙적으로 보면 조사대상업종과 사업체 규모의 확대가 필요할 것으로 판단되며, 업종과 규모를확대하기 위해서는 전체 표본크기 확대도 필요할 것임
+- 현행 표본설계에서 조사대상 업종과 사업체 규모를 제한한 것은 제한된 예산 하에서 효율적인 조사를 위해서 저임금 근로자의 비중이 높은 업종과 사업체규모를 중심으로 선정된 것임
+- 조사대상 사업체의 업종을 현행 조사와 마찬가지로 제한을 둘 것인지, 상용근로자 300인 미만의 규모로 제한을 둘 것인가의 문제에 대해서도 정책적인 판단이필요할 것임
+3. 표본크기, 층화, 표본배분, 가중치 산출 및 추정 관련
+○ 「최저임금 적용효과 실태조사」의 주요 조사 결과는 통계청 KOSIS를 통해 일부 문항에 대해 결과표를 제공하고 있음
+〇 이 조사의 통계작성 단위는 산업대분류 구분과 사업체 규모 구분임. 따라서조사대상 업종과 사업체 규모가 늘어나면 전체 표본크기가 늘어나는 것은 불가피할 것임
+- 업종별 통계작성이 필요하고 주요 공표항목이 모비율 추정이라는 점을 고려할 때 업종별 표본크기를 결정하는 것이 바람직할 것으로 판단됨
+〇 층화에 사용되는 변수로 업종 및 사업체 규모 구분을 사용할 수 있으며, 각 업종 내에서 사업체 규모별 표본배분 방법으로 제곱근 비례배분법을 적용하는 것은 타당한 것으로 판단됨
+- 각 업종 내에서 사업체 규모 구분에 대해서 제곱근 비례배분법을 적용함으로써 사업체 규모별 추정결과의 안정성을 높일 수 있을 것임
+〇 모집단 특성 추정의 정확성을 확보할 수 있는 적절한 가중치를 산출하여추정에 활용하는 방안은 적합함
+- 사업체 기준의 가중치와 근로자 기준의 가중치를 각각 산출하여 해당 조사항목에 대해서 가중치를 적용한 추정법을 적용하는 것이 바람직할 것으로 판단됨
+2)질문내용
+〇 최저임금 적용으로 인한 변화(고용, 이윤 등)를 질문하는 경우, 최저임금적용으로 인한 결과를 구별하기 어려움
+〇 ‘귀사’에 해당하는 질문과 ‘국가 전반적인 경영’에 해당하는 질문을 혼동하지 않도록 표현 제시 필요
+↳ ‘귀사’에 해당하는 질문은 질문표현에 ‘귀사에서는’ 등의 표현 명시
+2. 조사체계 변경안 검토
+2.1 현 조사체계 적정성 검토
+〇 49개 지방관서에서 실시계획 수립, 조사원 채용·교육·관리, 현장조사관리를 각각 수행하여 행정부담 과중 및 업무량, 조사의 정확성 측면에서 지역별 편차가 발생
+- 표본배분에 따라 지방관서별 업무부담 편차 발생(’21년 기준 최소 6개소, 최대 172개소)
+- 자료수집 결과 지방관서별 할당된 표본 대비 실제 회수된 조사표가 많은 지청이 ’20년 13개, ’21년 16개로 표본대체 지침을 미준수하고 있는 것으로 확인됨
+· 조사지침서에 따르면 저임금 근로자가 없거나 불응·불능으로 조사 불가능할 경우에 표본대체가 이루어져야 하므로, 조사성공 표본은 목표표본보다 작거나 같아야 함
+· 예비표본이 아닌 현장에서 섭외하여 조사한 표본으로의 표본대체는 조사자의 편의에 의해 조사된 표본이므로 대표성이 없음
+- 최근 3년 근로자조사의 목표 표본(10,000명)대비 회수 표본 평균 비율이 55.7%로 낮은편인데도 불구하고 회수한 조사표 중 분석 불가능한 조사표가 발생(11.3%)
+· 현장조사 후 별도 기관에서 전산입력, 전산처리를 시간을 두고 각각 따로 실시하여 응답의 정확성이나 성실도를 제대로 확인하기 어렵고 누락값에 대한 보완조사나 재조사도 잘 이루어지지 않음
+○(개선안)조사의 정확성을 높이기 위해 조사 관리를 철저히 하고 응답률을 높이기 위하여 아래와 같은 조사체계 개선이 필요
+- (행정 절차 간소화)각 지방관서별 각각 실시하는 계획수립, 조사원 채용·교육을 조사총괄 기관에서 일괄적으로 수행
+- (조사 효율화)근로감독관 업무 경감 및 체계적이고 일관적인 조사를 위해 근로감독관은 조사 진척률 관리 및 불응 사업체 조사 지원 업무를 담당하고, 전문 조사기관은 조사지침을 준수하여 현장조사를 실시하면서 응답률 제고를 위해 조사대상을 여러 번 접촉 필요(최소 2회 이상 방문, 조사관리자·담당공무원과 협력)
+· 전문 조사기관에서는 조사표 회수 후 바로 전산입력, 내용검토, 전산처리하고 필요시 보완조사를 실시하여 항목 무응답 및 분석 불가능 조사표를 최소화
+· 단, 이 경우 통계작성기관은 ‘통계청 훈령 제527호, 통계조사 민간위탁 관리 지침’에 따라 조사기관으로부터 조사원 교육 관련 사항(지침서, 사례집 등), 조사표 원본, 조사결과 원자료, 마이크로데이터 등 조사결과를 제출받아 관리하여야 함
+2.2 조사지침서 개선
+1)조사대상 근로자 선정 기준
+〇 조사 우선순위에 대한 기준이 모호하여 같은 사업체를 조사하더라도 조사원에 따라 다른 조사대상을 조사할 가능성이 높음
+- 고용형태별 근로실태조사 원자료(2020년 조사자료)에서도 개별 사업체별로 최저임금(8,590원)의 1.5배 이하에 해당하는 근로자의 수는 평균 7.88명으로 나타났고, 전반적으로 규모가 클수록 저임금 근로자 수가 많은 것으로 나타남
+〇(개선안)최저임금을 받는 평균 근로자 수는 상용 근로자 수 30~99명, 100~299명 구간에 많이 분포하므로 10~99명 구간을 10~29명, 30~99명으로 세분화한 후 30~299명 구간의 선정 가능한 근로자 수를 증가시키는 것을 검토하고 명확한 조사 우선순위 기준을 설정
+2)표본대체 지침
+〇 해당 표본은 산업대분류 및 사업체 규모로 층화되어 있으므로 표본대체는 동일한 층 내에서만 이루어져야 하나, 조사지침서 내에 수록된 표본 대체요령에서 다른 층과 표본 대체(3)를 하거나, 조사자가 임의로 표본추출틀외의 사업체 표본을 선정하도록 안내(4)하고 있어 조사된 표본의 모집단에 대한 대표성 문제가 발생함
+○(개선안)원표본 외 대체 표본을 준비하여 단위 무응답 발생 시 명확한 표본대체지침에 따라 표본 대체하여 조사
+- 원표본과 층화변수(산업대분류, 사업체 규모)및 정렬변수(시도, 시군구 등)가 동일하면서 가장 가까운 표본 활용
+- 표본 명부에서 대체 전 사업체에 대체유형에 해당하는 코드(전입, 휴업, 폐업, 소재불명, 대상외, 중복, 합병, 응답불응, 기타 등)를 입력하고 대체 후 명부에 몇 번째 대체 표본인지 표시
+- 조사 대상이 계속 응답을 거부하는 경우, 조사관리자·담당 공무원에게 보고하고, 최소 2회 이상 통화·방문하여 설득(조사관리자, 담당 공무원과 협력)
+* 응답회피, 상습적‧고의적 응답지연, 전화통화 회피(3회 이상)등 묵시적 거부의 경우 지방관서 담당 공무원이 판단하여 불응으로 처리 가능
+- 전체 목표 표본 수 보다는 층별 목표 표본 수를 유지할 수 있도록 표본을 관리
+제6장 결론 및 제언
+1.</t>
+  </si>
+  <si>
+    <t>○ 조사의 용이성
+- 조사 표본이 수월하게 확보될 수 있도록 설정되어야 함
+⇒ 각 기준들이 서로 상충될 수도 있음: 예를 들어, 국제적으로 통용되는 저임금근로자의 개념은 중위임금의 2/3 이하 임금근로자이지만(객관성 만족), 현재우리나라 상황에서는 최저임금이 중위임금의 2/3 수준에 도달한 상태이기 때문에 국제기준을 따를 경우 조사의 목적에 부합하는 조사대상을 충분히 포괄하지 못할 가능성이 있으며, 통계의 시계열적 안정성을 유지하지 못하게 됨
+1.2 조사대상 저임금 근로자 선정기준(안)
+1)제1안: 현행 유지 – 최저임금액의 1.5배 이하 근로자
+○ 근거
+- 현재까지 활용되어 왔던 기준 유지
+○ 장점
+- 통계의 시계열적 안정성을 확보할 수 있다는 점이 최대 장점임
+- 지금까지의 조사 경험을 활용할 수 있음
+○ 단점
+- 최저임금액의 1.5배가 중위임금에 가까워진 상황에서 최저임금액의 1.5배 근처의 임금근로자들이 과연 저임금 근로자에 부합하는 근로자인지에 대해서는 이견이제기될 수 있음
+- 조사대상 근로자의 포괄 범위를 최저임금과 연동시킬 경우 최저임금이 급격하게 변동하게 되면 조사대상 근로자의 포괄 범위도 크게 변동하게 되며, 최저임금의 1.5배가 중위임금을 넘을 가능성도 배제할 수 없음
+2)제2안: 중위임금(P50)이하 근로자
+○ 근거
+- 최저임금(인상)이 중위임금 이하 근로자들의 임금을 상대적으로(더 빠르게)증가시켜 임금격차(소득불평등)해소에 기여할 수 있다는 연구 결과(&lt;|start|&gt;#@이름1#&lt;|end|&gt;·&lt;|start|&gt;#@이름2#&lt;|end|&gt;, 2018;&lt;|start|&gt;#@이름3#&lt;|end|&gt;, 2011)
+- 최저임금이 인상될 경우 중위임금 이하 근로자들의 고용(근로시간으로 측정한)이 상대적으로 더 크게 감소한다는 연구 결과(&lt;|start|&gt;#@이름4#&lt;|end|&gt;·&lt;|start|&gt;#@이름5#&lt;|end|&gt;, 2018)
+○ 장점
+- 중위임금은 임금분포 상의 지표로서 국제적인 비교가 가능한 지표이며, 일반인들에게 쉽게 인식될 수 있는 지표임(즉, 객관성 기준에 부합)
+- 최저임금액과 연동시키는 현행 방식에 비해 통계의 변동성이 낮을 것으로 기대됨
+○ 단점
+- 중위임금 근처의 근로자들이 과연 저임금 근로자 개념에 부합하는지에 대해서는 이견이 제시될 수 있음
+- 최근에는 최저임금의 1.5배와 중위임금 간 격차가 상당히 줄어들긴 하였지만, 아직 완전히 일치하는 것은 아니어서 중위임금 이하 근로자까지 포함하는 방안의 경우 통계의 과거와의 시계열적 일관성을 완벽하게 확보할 수는 없음
+3)제3안: 중위임금의 2/3 이하 근로자
+○ 근거
+- 중위임금의 2/3 이하 근로자는 국제 비교(OECD)에서 널리 활용되고 있는 대표적인 저임금 근로자 개념임
+- 최저임금(인상)으로 인해 고용(근로시간)측면에서 부정적인 효과를 경험할 가능성이 있는 근로자는 최저임금 1.3배 이하의 저임금 근로자라는 연구 결과(&lt;|start|&gt;#@이름1#&lt;|end|&gt;, 2020)
+- 최저임금(인상)의 상대임금(증가)에 대한 효과가 임금분포의 하위 20분위에서 매우 강하게 나타난다는 결과(&lt;|start|&gt;#@이름2#&lt;|end|&gt;·&lt;|start|&gt;#@이름3#&lt;|end|&gt;, 2018)
+- 최저임금(인상)의 고용(근로시간)감소 효과가 임금분포의 하위 20분위에서 매우 강하게 나타난다는 결과(&lt;|start|&gt;#@이름4#&lt;|end|&gt;·&lt;|start|&gt;#@이름5#&lt;|end|&gt;, 2018)
+○ 장점
+- 저임금의 포괄 범위가 임금분포의 하위에서 협소하게 설정되므로 ‘저임금’ 근로자의 개념에 상대적으로 더 부합
+○ 단점
+- 현행 포괄 범위와 저임금의 범위가 상당히 상이하기 때문에 통계의 시계열적 안정성을 확보하기 어려움
+- 조사 모집단의 범위도 현재보다 축소되어 조사대상 표본추출에 어려움이 예상되고, 실제 조사에서도 저임금 근로자라는 ‘낙인효과’ 때문에 단위 무응답 및 항목무응답이 많을 것으로 예상됨
+2. 조사대상 업종 및 사업체 규모
+2.1 조사대상 업종
+○ 저임금 근로자는 모든 업종에서 존재하기 때문에 조사대상 업종을 거의 전업종으로(기존 10개 업종에서 17개 업종으로)대폭 확대하여 다양한 업종의 저임금 근로자들을 아우르는 통계를 작성한다는 취지 자체는 타당함
+○ 다만, 조사대상 업종의 범위를 확대하는 데 있어서는 업종마다 저임금 근로자 규모가 다르기 때문에 저임금 근로자 수가 적은 업종의 경우 조사대상 사업체 추출이나 모집단 추정이 어렵다는 현실적인 제약들을 고려할 필요가 있음
+○ 저임금 근로자의 기준을 달리할 때 업종별로 저임금 근로자의 비중이 어느 정도인지를 보여주고 있는데, 통상적인 저임금근로자 개념(중위임금의 2/3 이하)하에서의 저임금 근로자의 비중은 지난 10년 동안 거의 모든 업종에서 크게 감소한 반면, 중위임금 이하 또는 최저임금액의 1.5배 이하 근로자의 비중은 반대로 상당폭 증가하였음
+- 이는 최저임금의 인상 등으로 인해 우리나라 노동시장에서 임금분포가 지속적으로 압축되어 왔다는 것을 반영해 주는 결과임
+- 중위임금이나 최저임금액의 1.5배를 기준으로 저임금 근로자 비중을 살펴볼 경우 최근에는 업종간 저임금 근로자 비중의 격차가 상당히 줄어들고 있는 추세에 있음
+- 그럼에도 불구하고 기존 연구의 개선안에서 제안된'최저임금 적용효과에 관한 실태조사'의 조사대상 포함 업종에서(음영으로 처리된 업종들)의 경우 여전히 기존 조사대상 업종에 비해 저임금 근로자 비중이 상당히낮음
+○ 저임금 근로자들만을 대상으로 했을 때 이들의 산업분포를 나타낸 것임
+- 전체 저임금 근로자 중 기존 개선안에서 제안된'최저임금 적용효과에 관한 실태 조사'의 조사대상 포함 업종(음영으로 처리된 업종들)에 종사하는 저임금 근로자의 비중은 매우 낮음
+- 예를 들어, 광업, 전기가스업, 폐기물환경 등의 업종에서는 전체 저임금 근로자의 1% 미만이 종사하고 있고, 정보서비스, 금융보험업에 종사하는 저임금 근로자도 각각 전체 저임금 근로자의 2% 미만임
+2.2 조사대상 사업체 규모
+○ 현행 실태조사의 조사대상 사업체는 상용근로자 300인 미만의 사업체이며, 이들을 6개 범주(0인, 1~4인, 5~9인, 10~29인, 30~99인, 100~299인 등)로 나누어 통계를 작성하고 있음
+○ 조사대상 사업체 규모를 어디까지 설정하느냐의 문제 또한 정답이 있는 것은 아니며, 실태조사 초기에 300인 미만의 사업체로 한정한 이유는 다분히 저임금 근로자의 사업체 규모별 분포를 감안한 현실을 고려하여 결정한 것으로 보임
+○ 과연 300인 미만의 사업체로 한정하는 것이 현재에도 여전히 유효한지역시 현재 저임금 근로자의 사업체 규모별 분포와 연관지어 검토되어야 할것임
+○ 2021년 기준 산업별 및 규모별(저)임금 근로자 비중을 보여주고 있음
+- 최저임금의 1.5배나 중위임금 이하 근로자의 비중을 살펴보면, 규모별로는 300인 미만 사업체 범주까지는 그 비중이 대략 40% 또는 그 이상이며
+- 중위임금의 2/3 이하 저임금 근로자의 비중을 살펴보면 종업원 수 0인 사업체에서 그 비중이 압도적으로 높으며 이후 300인 미만 범주까지는 5% 이상을 보임
+- 다만, 중위임금의 2/3 이하 근로자를 저임금 근로자로 볼 경우, 다수의 업종에서 규모별로 10인 이상의 범주에서는 저임금 근로자의 비중이 2~3% 이하로 매우 낮음
+3.</t>
+  </si>
+  <si>
+    <t>표본설계
+3.1 모집단 및 표본추출틀
+○ 「최저임금 적용효과에 관한 실태조사」의 모집단을 전체 사업체로 확대하는 방안을 고려할 때 표본추출틀로 「사업체 노동실태현황」을 사용하는 것은 타당함
+- 조사대상 적정성에 대한 검토는 정책적인 활용 목적에 따라 이루어질 수 있으며, 표본설계에서 모집단 설정은 이를 반영하여 수정될 수 있을 것임
+3.2 조사대상 업종 및 사업체 규모 범위 확대
+〇 조사대상 업종의 확대가 필요할 것으로 판단됨
+〇 조사대상 사업체를 상용근로자 300인 미만의 규모로 제한을 둘 것인가의 문제에 대해서도 향후 정책적인 판단이 필요함
+3.3 표본크기, 층화, 표본배분, 가중치 부여 및 추정
+〇 이 조사의 통계작성 단위는 산업대분류 구분이며, 조사대상 업종이 확대되면 전체 표본크기도 늘어나는 것은 불가피함
+- 다만, 본 조사는 업종별 통계작성이 필요하고 주요 공표항목이 모비율 추정이라는 점을 고려하면 업종별 표본크기를 결정하는 것이 바람직할 것으로 판단됨
+〇 층화에 사용된 변수는 사업체의 업종과 사업체 규모 구분이며, 각 업종내에서 사업체 규모별 표본배분 방법으로 제곱근 비례배분법을 적용하는것은 타당한 것으로 판단됨
+〇 모집단 특성 추정에 대한 대표성과 정확성을 확보할 수 있는 적절한가중치를 산출하여 추정에 활용하는 방안은 적합함
+- 가중치는 사업체 가중치 및 저임금근로자 가중치를 구분하여 부여하여야 하며, 설계 가중치, 무응답보정 가중치, 사후층화조정 가중치를 포함한 최종 가중치를 적용하여 모수를 추정함
+4. 조사표 구성
 4.1 근로자 응답대상
 ○ 응답대상 검토 및 일치하도록 구성
 - 조사대상 근로자수는 ‘상용근로자 수’를 기준으로 하고 있으며, 사업체 대상 조사표는 일용/기간제 근로자를 포함하고 있으므로 응답대상을 검토 및 일치하도록 구성
@@ -156,97 +283,306 @@
 - 최저임금의 제시된 정보가 응답에 영향을 미칠 수 있기 때문에 현황표에 제시된 정보의 범위 검토
 〇 시간 흐름 순으로 응답란 제시 고려
 〇 응답대상이 달라지지 않는 문항은 독립질문으로 구성 필요
-〇 항목별 변동에 대한 응답과 최저임금으로 인한 영향을 혼합하여 응답할 가능성이 있으므로 질문을 구분하는 방안 필요</t>
-  </si>
-  <si>
-    <t>2)사업 추진경과
-○ 지원단체 선정
-사업공고 및 설명회를 통해 사업신청에 대한 홍보를 진행한 후 NPAS를 통해 지원 희망단체의 공익사업신청서를 접수받고, 이에 대한 평가(공익사업선정위원회)를 거쳐 최종 지원 사업을 선정함. 
-○ 교부신청 및 1차 교부금 지급
-지원단체를 대상으로 집행지침에 대한 교육과 실행계획서 컨설팅 진행 후 지침에 부합하도록 실행계획서 보완 진행, 최종적으로 1차 교부를 진행함. 
-○ 사업실행 및 집행
-단체가 계획한 단위사업에 따른 사업실행 및 그에 따른 예산집행을 보조금 교부 이후부터 12월 31일까지 진행함. 
-○ 교육 및 워크숍 진행
-단체들의 사업 이해도 향상과 역량강화를 위해 총 4회 역량강화교육 및 2회 워크숍을 진행함. 2020년의 경우 코로나19로 대면회의가 어려워짐에 따라 워크숍과 모든 교육을 온라인으로 진행함. 
-&lt;워크숍 및 교육 추진현황&gt;
-○ 중간평가 및 2차 교부금 지급</t>
-  </si>
-  <si>
-    <t>◯ 8개 우수단체 모두 회계평가 전 영역에서 우수 등급을 받음. 회계평가 우수단체의 경우 정산자료 증빙에서부터 집행률, 계획변경 및 집행 적법성, 전자증빙, 실적 대비 사업비 집행에 있어서까지 회계 전 과정에서 우수하게 진행된 것으로 나타남. 
-◯ 회계평가 결과 가장 점수가 낮은 하위 2개 미흡단체는 4유형에 2개가 분포되어 있음. 이들 2개 미흡단체 모두 보조금 집행등록 평가에서 부적정 비율이 높아 보조금 사용 적법성 부분에서 모두 미흡으로 평가됨. 
-◯ 정산자료 구비 적절성의 경우 집행등록 평가에서 부적정 평가를 받은 단체들의 다수가 정산자료 구비 상태가 미흡한데에서 기인함에 따라 해당 지표에서 미흡등급을 받게 됨. 
-◯ 또한, 이들 단체들의 경우 집행 15일 내 등록 기준을 충족시키지 못하는 집행등록 건수가 많아서 집행등록 지연비율 항목에서 미흡 또는 보통으로 평가됨. 
-&lt;회계평가 결과 하위 2개 미흡단체&gt;
-2. 사업유형별 평가결과
-1)유형별 평가결과 종합</t>
-  </si>
-  <si>
-    <t>&lt;워크숍 및 교육 추진현황&gt;
+〇 항목별 변동에 대한 응답과 최저임금으로 인한 영향을 혼합하여 응답할 가능성이 있으므로 질문을 구분하는 방안 필요
+〇 우선적으로 고려할 사항을 질문하는 항목은 복수응답 개수를 제한하여순위 질문으로 변경하는 방안 검토 필요함
+〇 최저임금과 직접 관련된 내용으로 보이지 않은 항목 검토 필요함
+〇 문항 배치 검토 필요
+〇 가구 전체 소득 및 지출금액으로 최대범위(500만원 이상)가 다소 적은것으로 보이므로 검토 필요함
+〇 사업장의 고지 여부를 근로자에게 질문하는 것이 적절한지 검토 필요함
+5. 조사체계
+○ 조사의 정확성과 효율성 제고를 위해 그동안 각 지방관서별로 이루어졌던조사계획 수립, 조사원 채용 및 교육 등을 조사 전문기관에서 일괄적으로수행
+- 근로감독관은 조사 불응 사업체에 대한 조사 지원 업무를 담당하고 조사기관은 조사대상에 대한 현장조사를 강화하여 응답률 제고
+○ 최저임금 근로자가 상대적으로 많이 분포하는 기업규모 군에 대해 선정가능한 근로자 수를 증가시킬 수 있도록 조사의 우선순위 기준 명확화
+○ 업종별·규모별로 충분한 수의 예비표본을 확보하여 단위 무응답 발생 시명확한 표본대체지침에 따라 표본 대체하여 조사
+- 원표본과 층화변수(산업대분류, 사업체 규모)및 정렬변수(시도, 시군구 등)가 동일하면서 가장 가까운 표본 활용
+- 전체 목표 표본 수뿐만 아니라 층별 목표 표본 수를 유지할 수 있도록 표본을 관리
+『여성농업인실태조사』품질개선 컨설팅 최종결과보고서
+Final Report on Quality Improvement Consulting for 『Survey on the Korean Women Farmers』
+한국조사연구학회
+2022.8. 최종결과보고서 요약문
+여성농업인실태조사는 여성농어업인육성법 제8조, 통계법 제18조에 의한 승인통계(제114036호)에 조사 근거를 두고 있다. 2018년 여성농업인실태조사를 검토한 결과‘표본 규모 확대’, ‘표본설계 개선’, ‘유사통계 비교’, ‘조사표 설계’ 등이 필요한 것으로파악되었다. 이에 본 연구에서는 2018년 여성농업인실태조사의 표본설계 및 조사결과를 바탕으로 새로운 표본설계 방안을 연구하여 통계 신뢰성 제고를 위한 적정 표본크기를제시하는 한편, 조사대상 확대 가능성에 대해 검토하고, 유사통계와 조사표 조사항목의 적정성 등을 검토하여 여성농업인실태조사의 품질개선 방안을 마련하고자한다. 본 연구의 주요 결과를 정리하면 다음과 같다. 첫째, 여성농업인실태조사의 조사단위 및 조사대상의 적정성을 검토하고, 통계청에서작성 및 관리하고 있는 2020년 농림어업총조사를 표본추출틀로 사용하여 확률표본추출하는 표본설계 방안을 제시하였다. 통계 신뢰성을 제고하기 위해 조사모집단 즉여성농업인을 충분히 대표할 수 있는 적정 표본규모를 제시하는 한편, 지역(9개 도및 특광역시)및 동/읍면부를 층화기준으로 사용하여 모집단의 특성을 잘 반영한효과적인 표본배분방법을 검토하고, 정확한 통계산출을 위하여 표본설계에 따른모수추정식, 가중치 산출 등을 포함한 새로운 표본설계 방안을 제시하였다. 둘째, 농어업인 등에 대한 복지실태조사, 다문화가족실태조사, 양성평등실태조사 등유사통계의 조사대상 범위 및 조사내용, 표본규모 및 예산 등 작성현황을 비교분석하였다. 마지막으로, 조사목적에 부합하는 조사표 설계방법의 적정성을 검토하고, 조사대상별조사표(일반여성농업인, 귀농여성농업인, 다문화가정여성)의 조사항목간 중복, 활용도및 중요도, 개별문항 등을 검토하여 조사항목을 정비하고 조사표 개선안을 제시하였다. 요약
+여성농업인실태조사는 여성농업인에 대한 전반적인 현황을 파악하는 객관적이고 신뢰성 있는 데이터를 구축하여 통계 이용자 수요에 부응하고, 정부, 산업계, 학계 등 여성농업인 육성 5개년 계획의 중간평가 및 관련 정책수립을위한 기초자료로 활용하는 데 그 목적이 있다. 2020년 여성농업인실태조사 정기통계품질진단 결과 및 표본설계를 검토한결과 ‘표본규모 확대 및 표본설계 개선’, ‘유사통계 검토’, ‘조사표 설계 및 조사항목 개선’ 등이 필요한 것으로 파악되었다. 따라서 본 연구에서는 2018년 여성농업인실태조사의 조사결과와 기존의 표본설계를 바탕으로 새로운 표본설계 방안과 그에 적절한 모수 추정방안, 조사 목적에부합하는 조사표 및 조사항목 등 조사표 설계 개선안을 마련하여 여성농업인실태조사의 품질개선 방안을 제시하였다. 현재 여성농업인실태조사는 일반여성농업인, 귀농여성농업인, 다문화가정여성을대상으로 각각 별도의 조사표와 조사항목을 사용하여 여성농업인의 실태를 조사하고 있는데, 조사대상별 표본설계와 표본설계 개선안을 비교하여 요약하면다음과 같다. 결론적으로 새로운 표본설계에서는 일반여성농업인과 귀농여성농업인 실태조사를 통합하고, 지역을 층화기준으로 구축된 조사모집단에 대한 충분한 분석을 통해모집단의 특성을 잘 반영한 효과적인 표본배분방법과 표본추출방법을 제시하였다. 또한 정확한 통계산출을 위해 표본설계에 따라 설계가중치와 조사과정에서 발생하는 무응답 조정을 위한 무응답조정가중치 등을 적용한 가중치를 부여하는 과정을구체적으로 기술하였고, 모수추정식을 제시하였다. 다문화여성실태조사는 조사목적에 적합하지 않아 조사대상에서 제외하였다. 제 1 장 서 론
+제 1 절 연구배경 및 목적
+‘여성농업인실태조사’는 여성농업인에 대한 전반적인 현황을 파악하는 객관적이고 신뢰성 있는 데이터를 구축하여 통계 이용자 수요에 부응하고, 정부, 산업계, 학계 등 여성농업인 육성 5개년 계획의 중간평가 및 관련 정책수립을위한 기초자료로 활용하는 데 그 목적이 있다. 이 조사는 여성농어업인육성법제8조, 통계법 제18조에 의한 승인통계(제114036호)에 조사 근거를 두고 있다. 본 조사는 2003년 여성농업인실태조사로 최초 실시된 이래, 5년 주기로 조사가 실시되어 2018년 제4차 실태조사가 완료되었다. 2003년 국가승인통계로 지정되었으며, 조사기간, 표본설계 변경, 조사항목 수정 등의 이유로, 2008년, 2014년, 2018년 통계작성 변경승인을 받은 바 있다. 여성농업인실태조사는 조사원이 직접 가구를 방문하여 조사하는 면접조사로 2018년 조사의 조사 실시 기간은 2018.8.28. ~ 2018.10.12이고 조사 기준시점은 2017.9.1. ~2018.8.31.</t>
+  </si>
+  <si>
+    <t>2021년 「최저임금 적용효과에 관한 실태조사」의 작성승인사항, 표본설계 내역 및 조사결과를 검토한 결과 ‘조사대상 선정 기준 검토’, ‘조사체계 변경 필요성’ 및 ‘조사방법 개선안 제시’ 등이 필요한 것으로 파악되었다. 따라서 본 연구에서는 2020~2021년 「최저임금 적용효과에 관한 실태조사」의 선행 연구, 조사결과와 기존의 표본설계를 바탕으로 조사목적에 맞는 조사대상 기준, 조사표 설계, 조사체계 및 조사방법의 적절성 등을 검토하고, 표본설계 전문가 자문회의를 통해 「최저임금 적용효과에 관한 실태조사」의 품질 개선 방안을 제시하였다. 본 연구에서 도출된 결과 및 제언들은 다음과 같다. 첫째, 「최저임금 적용효과에 관한 실태조사」는 조사대상 사업체와 근로자에 대해 ‘최저임금액의 1.5배 이하를 받는 저임금 근로자와 이들을 고용하는 사업주’로 설정하고 있는데, 향후 조사에서는 조사대상 근로자에 대한 보다 명확하고 합리적인 기준 설정이 필요한 것으로 판단된다. 그동안 최저임금이 지속적으로 상승하면서 최저임금의 1.5배가 최근에는 거의 중위임금 수준까지 다다른 상황에서 현행 조사대상 근로자 선정 방식을 유지하는 것에 대한 검토가 필요하다는 것이다. 본 연구에서는 최저임금(인상)이 임금분포 상에서의 근로자들의 임금과 고용에 미치는 영향에 대한 실증 연구의 결과를 토대로 조사대상 근로자를, 1)현행대로 최저임금의 1.5배 이하 근로자로 설정하는 방안, 2)중위임금 이하 근로자를 조사대상으로 삼는 방안, 3)중위임금의 2/3 이하 근로자를 조사대상으로 삼는 방안 등 세 가지 안을 제시하였다. 현행 방식을 유지하는 방안은 통계작성의 일관성을 유지할 수 있는 장점이 있는 반면에 최저임금이 지속적으로 상승할 경위 최저임금의 1.5배가 중위 임금을 넘어설 가능성이 있어 조사대상 ‘저임금’ 근로자에 대한 논란이 지속될 수 있다. 중위임금 이하 근로자를 조사대상 근로자 선정기준으로 삼는 방안은 중위임금이 임금분포 상에서의 지표이기 때문에 쉽게 이해할 수 있고 최저임금의 변동과 상관 없이 일정 수준(전체 근로자의 절반)의 근로자들을 조사대상으로 삼기 때문에 조사대상 모집단의 일관성 유지 측면에서 이점을 가지는 방안이다. 중위임금의 2/3 이하 근로자를 조사 대상으로 삼는 방안은 중위임금의 2/3 이하가 국제적으로 통용되는 통상적인 저임금 근로자의 정의에 부합한다는 점에서 장점이 있는 반면, 현행 방식 보다 포괄되는 조사대상이 협소하게 됨에 따라 조사대상 사업체 및 근로자 추출에 있어 현실적이 어려움이 클 것으로 예상된다. 이들 각 방안의 장단점 들을 고려하여 현실에 맞는 조사대상 근로자 선정 방안이 정책적으로 결정될 필요가 있다. 둘째, 현재 10개 업종에 대해 조사하고 있는 업종의 포괄 범위를 17개 업종으로 확대하여 더 다양한 업종에서 최저임금 관련 인식을 조사하는 것은 바람직한 것으로 평가된다. 실제로 저임금 근로자들은 다양한 업종에서 종사 하고 있는 것이 사실이며, 업종의 폭을 넓혀 조사할 경우 보다 종합적인 인식조사가 가능해질 수 있다. 다만, 저임금 근로자의 산업별 분포를 살펴 보았을 때 일부 업종에서는 상대적으로 상당히 적은 수의 저임금 근로자만 종사하고 있어 이들 업종에서 조사대상 사업체와 저임금 근로자를 확보하기가 현실적으로 쉽지 않을 가능성이 있다. 따라서 조사의 포괄 업종 결정 시 조사의 수월성도 고려하여 점진적으로 확대해 나가는 것이 합리적인 것으로 판단된다. 같은 논리로, 조사대상 기업체 규모(현재는 0인부터 300인 미만 사업체들에 대해 조사)를 확대하는 문제도 조사의 현실적 어려움까지 감안 하여 결정할 필요가 있다. 셋째, 표본추출 틀은 현재와 같이 고용형태별근로실태조사와 사업체노동실태 현황을 활용한 2중 추출 형식으로 가는 것이 불가피한 상황인 것을 보인다. 고용형태별근로실태조사를 통해 업종별 및 규모별 저임금 근로자의 분포를 파악하고 사업체노동실태현황의 사업체 리스트를 활용하여 조사대상 사업체 및 근로자 그리고 대체표본들을 확보하는 것이 합리적인 것으로 판단된다. 넷째, 현재 업종 및 기업규모를 기준으로 비래배분하고 있는 표본배분 방식을 제곱근 비례배분으로 변경하고, 표본오차를 고려하여 사업체 조사목표 표본수를 현행 3,000개에서 3,500개로 확대하며, 업종 및 기업규모 등의 층화를 바탕으로 가중치를 적용함으로써 모수 추정이 가능하도록 해야 할 것으로 보인다. 다섯째, 조사표의 구성과 관련하여 조사대상 근로자수는 ‘상용근로자 수’를 기준으로 하고있는 반면 사업체 대상 조사표에서는 일용/기간제 근로자까지 포함하고 있는 상황이어서 응답대상을 일치시키도록 할 필요가 있으며, 근로자 응답대상자 선정과 구분이 용이하도록 사업체 조사표에서 관련 정보가 도출 되도록 할 필요가 있다. 아울러 사업체의 정보 확인 및 기타 행정자료 연계를 위해 사업체 조사표에서 사업자등록번호가 추가되도록 하며, 시간 흐름 순으로 응답란이 제시되도록 할 필요가 있다. 마지막으로, 그동안 고용노동부 지방관서의 근로감독관 주도 하에 임시 조사원을 통해 조사되었던 조사체계를 조사 전문기관이 보다 체계적으로 조사하도록 변경하는 것은 바람직한 방향으로 판단된다. 이러한 조사체계의 변경은 근로감독관의 부담을 경감시키고, 조사원 채용/교육/관리 측면에서 상대적으로 전문성을 보유한 전문 조사기관이 담당함으로써 조사의 효율성을 제고할 수 있을 것으로 기대된다. 다만, 조사체계 변경 시에도 기업체들로 하여금 조사에 협조할 수 있도록 근로감독관과의 협력이 요청되며, 조사 불응 또는 비협력 사업체들에 대해 근로감독관이 조사지원 업무를 수행하는 것은 불가피할 것으로 보인다. 제1장 서론
+1. 연구목적
+- 「최저임금 적용효과에 관한 실태조사」는 저임금근로자를 고용하고 있는 사업체의 사업주와 근로자를 대상으로 최저임금 결정수준 등에 대한 인식을 매년 조사하여 최저임금 심의의 기초자료로 활용되어 왔음
+- '최저임금 적용효과에 관한 실태조사'는 저임금근로자를 고용하고 있는 사업체의 사업주와 근로자를 대상으로 최저임금이 기업경영과 고용에 미치는 효과, 사용자와 근로자가 실제 느끼는 최저임금 수준의 만족도 등을 조사하여 최저임금 심의의 기초 자료로 활용되고 있음
+- 본 조사는 1년 주기 조사로 매년 11월에 조사되고 있으며, 조사는 고용노동부 지방관서에서 수행하고, 전산입력 및 처리, 결과 분석 등은 외부 연구기관에서 수행하고 있으며, 최종적인 통계관리는 고용노동부 최저임금위원회에서 담당하고 있음
+- 본 조사는 최저임금법 제23조 및 시행령 제19조에 근거하고 있으며, 2007년에 국가승인통계로 지정된 후 당해 연도부터 매년 조사·작성되고 있음
+- '최저임금 적용효과에 관한 실태조사'의 조사대상 사업체의 범위는 저임금근로자가 밀집해 있는 제조업, 도·소매업 등 주요 10개 업종의 상용근로자 300인 미만 3,000여 개 표본 사업체이며, 동 사업체에 종사하는 사업주와 최저임금 시급액의 1.5배 이하의 10,000명 내외의 표본근로자를 대상으로 면접조사를 통해 자료를 수집하고 있음
+- 조사항목으로는 최저임금 인상의 영향, 최저임금 결정 시 고려사항, 최저임금액 수준에 대한 생각, 최저임금 인상률의 적정수준 등이 사업주와 근로자 대상 조사에 공통적으로 포함되며, 이들 이외에 사업주의 경영상황과 근로자의 기본 사항이 조사됨
+- 그러나 저임금근로자 고용 사업체의 모집단 설정이 불명확하여 조사된
+표본을 통해 의미 있는 통계를 작성하기가 어렵다는 지적이 제기되어 왔고, 이에 따라 최근 동 조사의 통계품질 개선을 위한 연구를 진행하여 개선안이 제시되었음
+- '최저임금 적용효과에 관한 실태조사'의 현행 조사 모집단은 ‘상용 300인 미만 사업체 중 최저임금액의 1.5배 이하를 받는 근로자와 이들을 고용하는 사업주’로되어 있으나, 저임금 근로자에 대한 규정이 명확하지 않고, 최저임금의 1.5배 이하 범위로 설정된 임금수준의 적절성에 대해서도 검토가 필요함
+- 모집단 설정과 더불어 표본추출 방식, 표본의 크기, 가중치 등 표본에 대한 설계도 기존 연구에서 제시된 바 있음
+○ 이에 본 연구에서는 모집단 설정, 표본설계 등과 관련하여 제시된 개선안의 적절성을 점검하되, 특히 조사대상인 ‘저임금 근로자’의 설정기준과 관련한 다양한 분석을 통해 합리적인 조사대상 모집단 설정을 도모하고 통계의품질 개선에 기여하고자 함
+2. 연구내용
+○ 기존 연구에서 제시된 「최저임금 적용효과에 관한 실태조사」의 통계품질 개선방안 고찰
+- 「최저임금 적용효과에 관한 실태조사」 개선방안 연구(2020)
+- 「최저임금 적용효과에 관한 실태조사」 표본설계 및 추정방안 연구(2021)
+○ 조사 모집단(조사대상 저임금 근로자)설정 기준 연구
+- 최저임금(인상)의 임금격차(불평등)완화 효과에 대한 기존 연구 분석
+- 최저임금(인상)이 고용에 미치는 영향에 대한 기존 연구 분석
+- 임금분포 상 어떠한(저임금)근로자 집단이 최저임금(인상)에 영향받는지 파악
+○ 표본설계 개선안 진단
+- 표본추출틀
+- 표본배분
+- 표본 크기
+- 가중치 부여
+- 층화
+○ 조사체계의 변경에 따른 문제점 점검 및 개선안 연구
+- 지방관서 근로감독관과 기간제 조사원의 현장조사 → 지방관서 근로감독관과 전문 조사업체에 의한 현장조사
+- 담당업무에 있어 근로감독관과 전문 조사업체 간 역할 조정
+3. 연구방법
+○ 「최저임금 적용효과에 관한 실태조사」의 통계품질 개선 관련 기존 문헌 고찰
+○ 조사대상 저임금 근로자 설정 기준 연구
+- 저임금 근로자의 정의 및 실증연구
+- 최저임금(인상)적용 임금분포 분석
+- 중위임금 대비 최저임금의 배율 추이 분석
+- 최저임금 인상의 영향을 받는 임금분위 분석
+- 전문가 자문
+○ 표본설계 개선안 진단
+- 기존 품질개선 연구에서 제시된 표본설계 관련 개선안의 적절성 진단
+○ 조사체계의 변경에 따른 문제점 점검 및 개선안 연구
+- 조사 담당자, 자료 분석 담당자 등 면담 조사
+제2장 선행 연구 검토
+1. 현행 최저임금 적용효과에 관한 실태조사의 틀
+1.1 조사체계
+○ 현행 최저임금 적용효과에 관한 실태조사(이하 실태조사)는 지방관서의 근로감독관의 주관 하에 임시 조사원들에 의해 현장 조사되고 있으며, 전산입력 및 처리, 그리고 결과분석 및 보고는 연구기관에서 수행
+1.2 조사 모집단
+○ 조사 모집단은 상용근로자 300인 미만의 사업체 중 최저임금액의 1.5배 이하를 받는 근로자와 이들을 고용하는 사업주임
+1.3 표본추출틀
+○ 고용형태별 근로실태조사와 사업체노동실태현황조사를 활용한 2중 추출
+- 고용형태별 근로실태조사로부터 산업·규모별 저임금 근로자 분포 정보를 추출한 후 사업체노동실태현황조사에 적용하여 조사대상 사업체 추출
+1.4 표본의 크기
+○ 현행 실태조사의(목표)표본의 크기는 사업체의 경우 3,000개이고, 근로자의 경우 이들 사업체에 종사하는 저임금 근로자 10,000명
+○ 2020년의 조사의 경우 추출된 2,857개소의 사업체 표본을 다음과 같은기준에 따라 조사함
+· 4인 이하 : 사업체당 최대 4명
+· 5 ~ 9인 : 사업체당 최대 5명
+· 10 ~ 99인 : 사업체당 최대 7명
+· 100 ~ 299인 : 사업체당 최대 10명
+1.5 층화
+○ 산업대분류 기준 10개 업종과 종사자 규모를 기준으로 한 6개 집단의교차 셀로 층화가 이루어짐
+- 10개 업종에는 제조업, 도매 및 소매업; 운수업; 숙박 및 음식점업; 부동산 및 임대업; 사업시설관리 및 사업지원 서비스업; 교육 서비스업; 보건업 및 사회복지서비스업; 예술, 스포츠 및 여가 관련 서비스업; 협회 및 단체, 수리 및 기타 개인서비스업 등이 포함됨
+- 사업체 규모는 상용근로자 수를 기준으로 0인, 1~4인, 5~9인, 10~29인, 30~99인, 100~299인 등의 6개로 분류됨
+1.6 표본배분
+○ 현행 실태조사 표본배분 방식은 단순 비례배분에 기초하고 있음
+1.7 공표범위
+○ 실태조사에서 제공되고 있는 통계표는 산업별(10개)및 규모별(6개)로작성되고 있으며, 원자료는 공개되지 않고 있음
+1.8 가중치
+○ 현행 실태조사는 모집단 설정이 불명확하여 가중치 적용이 불가한 상황임
+- 즉, 현행 방식에서는 저임금 근로자를 고용하는 사업체의 전체 명부가 존재하기 않기 때문에 모집단 추정을 위한 가중치 적용이 불가능함
+1.9 조사항목
+○ 최저임금액의 1.5배 이하를 받는 근로자와 이들을 고용하는 사업주 각각에 대해 각 20문항 내외 조사
+- 공통 조사내용:
+최저임금 인상률의 적정성 여부 및 판단기준, 내년도 최저임금 인상률 수준 등
+- 사용자 조사내용:
+사업체특성, 경영여건(매출액 등), 근로자특성별 고용규모, 최저임금으로 인한고용조정 여부, 고용사유, 임금인상에 미친 영향, 임금대비 생산성 수준 등
+- 근로자 조사내용 :
+인적속성(성, 연령, 학력, 직종 등), 가구특성(가구원수), 고용형태, 현 직장의 임금 등
+2. 표본설계의 특징
+○ 저임금 근로자를 고용하고 있는 사업체를 모집단으로 구성하여 표본추출을 하여야 하나, 이러한 추출틀은 존재하지 않으며, 만일 전체 사업체를대상으로 확률추출법을 적용하는 경우 다음과 같은 문제점이 발생
+- 조사대상 중 저임금 근로자 고용 사업체는 일부만 파악되어 조사의 효율성이 저하됨
+- 저임금 근로자 고용 사업체는 산업대분류와 사업체 규모에 따라 치우치는 경향이 있는데 과도한 조사비용이 소요될 수 있음
+○ 차선책으로 저임금 근로자들을 고용하고 있는 사업체에 대한 대략적인모집단틀을 구성하여 표본추출을 할 수 있으나 이 경우 조사의 효율성은 다소 높아지지만, 여전히 산업대분류와 사업체 규모의 분포를 반영하지못하는 조사결과를 얻게 됨
+- 이러한 조사상의 어려움을 줄이고자 고용노동부의 「사업체노동실태현황」 자료와 「고용형태별 근로실태조사」 자료를 근거로 하여 모집단 현황을 파악하고, 이로부터 산업대분류와 사업체 규모에 따른 표본 수를 결정함
+- 이 때 산업분류는 산업대분류 기준으로 상위(사업체 수)10개 영역으로 하고, 사업체 규모는 299인 이하인 사업체를 대상으로 하여 6개 규모로 함
+3. 선행 연구 검토 및 선행 연구에서 제시된 주요 항목별 개선안
+3.1 선행 연구 검토
+3.1.1 최저임금 적용효과에 관한 실태조사 개선방안 연구(2020)
+1)표본설계의 대표성 확보
+○ 표본설계에서 모집단(조사대상)의 설정
+- 「최저임금 적용효과에 관한 실태조사」 모집단(조사대상)의 최저임금 적용 효과 평가에의 적절성에 대한 전문가들의 평가는 다음과 같음
+- 현행 유지: 저임금 근로자를 특정하고 모집단으로 구성한 것은 적절함. 다만 모집단의 개념과 관련하여 목표모집단과 조사모집단에 대한 명확한 정의 기술 필요
+○ 조사대상 업종 및 대상 확대
+- 조사대상 업종의 확대: 저임금 근로자가 집중된 산업에서 저임금 근로자가 집중된 사업체를 선정하여 해당 산업 및 사업체의 저임금 근로자와 사용자에게 설문을 진행하는 현행 방식으로, 조사 결과에서의 저임금 근로자의 특성은 경제 전체에서의 최저임금 수급자와 차이가 있음. 본 조사의 결과를 전국 단위로 적용되는 최저임금의 심의자료로 활용하기 위해서는 전체 산업별, 사업체 규모별, 사업체 수 및 피고용인의 수를 고려하여 표본설계후, 저임금 근로자가 있는 사업장에 대해 진행하되, 저임금 근로자가 없는 사업장의경우 없다는 것을 표본에 대한 기초통계에 제시
+- ‘영세·소규모 사업장에 대한 영향 분석’ 혹은 ‘전체 사업장에 대한 영향 분석’으로 목적을 구분하고, 그에 맞는 모집단의 범위 설정 필요
+- 본 조사를 가능한 전체 업종별 규모별 분포를 볼 수 있도록 할 경우, 저임금 근로자가 충분히 표집될 수 있도록 하려면, 표본규모가 커져야 하는 등의 문제가 예상되므로 ① 일반국민 인식조사 ② 사업주 및 근로자 심층면접조사 ③ 근로자 임금실태조사 등의 부가조사를 통해 결과 보완 필요
+2)표본 규모의 적절성
+○ 「최저임금 적용효과에 관한 실태조사」의 표본 규모 및 표본 할당의 적절성에 대한 전문가들의 평가는 다음과 같음
+- 통계적으로 최소한의 신뢰성이 보장되는 규모로 표본확보(각 셀별 최소 32개 표본), 최소 2,000에서 최대 4,000개소 정도의 사업체에 대해서 설문 진행. 이 경우 시간 및 조사 비용 발생으로 60×32=1,920인 2,000여개소 정도를 추출
+- 조사대상 업종을 전산업으로 확대. 사업체 규모도 현재 1~4인에 집중하기 보다는 좀 더 다양한 사업체 규모의 표본 확대
+- 사업체 규모 100~299인은 늘 통계적 유의성 문제에 걸림. 표본을 약간 늘리고, 사후 가중치로 조정
+- 산업별 최소 표본(총합 기준)을 100개 이상으로 하고, 30인 이상 사업체에 대한 표본 수 확대. 분석 항목을 30~99인과 100~299인으로 구분하기보다 30인 이상으로 분류하는 방안도 의미가 있을 것임
+- 본 조사의 결과는 세부 셀의 사례수의 한계로 일반화 어려움. 따라서 사업체는 산업대분류별, 근로자 규모별로 분석 가능한 수준으로 근로자는 성별, 연령별, 학력별, 소득별, 고용형태별, 직업별, 소속 사업체 산업별 분석 가능한 수준으로확대 필요
+3)표본설계 관련 주요 개선 방향
+○ 저임금 근로자를 특정하고 모집단으로 구성한 것은 적절함. 다만, 모집단의개념과 관련하여 목표모집단과 조사모집단에 대한 명확하게 정의하는 것이 필요
+○ 조사대상 업종 및 대상 확대가 필요함
+○ 조사대상 업종을 전산업으로 확대할 필요가 있으며, 사업체 규모도 현재1~4인에 집중하기보다는 다양한 사업체 규모로 확대됨에 따라 전체표본크기의 확대가 필요함
+3.1.2 최저임금 적용효과에 관한 실태조사 표본설계 및 추정방안 연구(2021)동 연구에서 제안된 표본설계 방안의 주요한 결과를 요약하면 다음과 같음
+1)조사대상 확대
+○ 업종 확대 및 근로자 확대는 최저임금위원회 본 회의에서 최종적으로 결정해야 할 사항이지만 본 조사에서는 현행 10개 산업은 17개 산업으로, 최저임금 근로자를 저임금근로자로 확대하는 방안도 포함하여 검토하였음
+- 저임금근로자를 포함함으로써 사업체별 저임금근로자의 최저임금 적용효과를 파악하고, 저임금근로자와 최저임금 근로자의 비교를 통해 최저임금 적용 효과를 확인할 수 있도록 검토하였음
+2)표본추출틀
+○ 적절한 표본추출틀 확보를 위해 사업체노동실태현황(고용노동부), 기업통계등록부(통계청), 고용보험 DB(한국고용정보원)를 비교하여 최저임금 적용효과 실태조사의 조사 대상에 대한 최신성, 포괄성 및 고용노동부 내 다른 통계와의 정합성 등을 고려하여 사업체노동실태현황 사업체 명부로 설정함
+3)표본크기 결정
+○ 2020년 조사 결과 자료를 활용하여 사업체 수 및 근로자 수의 표본크기를 결정함
+- 사업체 수의 표본크기는 “저임금 종사자 수”, “시간당 임금”에 대한 전국 기준, 업종별 기준, 가중/비가중 등의 추정 결과에 대한 상대표준오차를 이용하여 약3,500개 사업체로 결정함
+- 이는 10개 산업을 17개 산업으로 확대하는 것과 사업체 내 저임금근로자 수의 확보 등을 고려하여 현행 조사의 표본 사업체 수 3,000개보다 500개 사업체를증가한 것임
+○ 사업체 내 조사 대상 근로자 수의 표본크기는 현행과 같이 10,000명을목표로 설정함. 이를 고려하여 본 과제에서는 업종별 및 사업체 규모별추정의 신뢰성 제고를 위해 업종별, 사업체 규모별 확보해야 할 최소 목표표본크기를 제시하였음
+4)층화변수
+〇 2020년 조사 결과 자료를 활용하여 “저임금 종사자 수”, “시간당 임금”, “월평균 임금” 등의 주요 변수를 이용하여 층화변수로 사용한 업종과 종사자규모에 대해 분산분석을 실시하여 현행 표본설계에서 사용하는 업종과종사자 수 규모의 층화변수가 적절함을 확인함
+5)표본배분 방법
+○ 본 과제에서는 기존 10개 업종 및 17개로 업종을 확대할 때의 표본배분을 모두 검토하여 제공하였음
+○ 조사 대상 사업체를 결정할 때 전체 사업체 및 임시일용근로자가 근무하는 사업체를 검토하여 전체 사업체를 기준으로 표본을 배분함
+○ 층화추출법에서 널리 사용하는 기본적인 표본배분방법(비례배분, 제곱근비례배분, 우선할당 후 비례배분)별로 기대표본오차를 산출해 비교하여 제곱근 비례배분방법으로 업종별, 사업체 규모별 표본크기를 배분함
+6)사업체 내 저임금근로자의 표본추출
+○ 사업체 내 저임금 근로자를 추출할 때, 사업체 저임금근로자의 대표성을확보할 수 있는 방안을 마련하기 위해 저임금 근로자 명부가 있는 경우와 없는 경우로 구분하여 근로자 추출 방안을 제안함
+○ 기본적으로 근로자의 성별, 연령대, 직급, 근속연수, 부서 등의 직무분야 등 근로자의 인구통계학적 특성 및 근무 특성을 반영하여 추출하는 방안을 제안하였음
+7)가중치 및 추정식
+○ 새로운 표본설계에서는(최)저임금 근로자가 근무하는 국내 사업체와(최)저임금 근로자의 최저임금 적용효과를 파악할 수 있고, 표본의 대표성을 확보하여 모집단 특성 추정의 추정 오차 최소화를 통해 정확성을 확보할 수 있는 적절한 가중치를 산출하는 방안을 제시하였음
+3.2 선행 연구에서 제시된 주요 항목별 개선안 정리
+3.2.1 조사체계
+○ 지방관서 근로감독관의 주도 하에 조사원들을 통해 조사되고 있는 현행 조사체계는 실사의 전문성과 효율성 제고를 위해 전문 조사업체에 의한 체계적인 조사로 변경할 필요가 있다는 의견이 제시됨(한국조사연구학회, 2020)
+○(개선안)조사업체가 ‘현장조사, 전산입력, 전산처리’를 일괄 수행하고 ‘결과분석’은 연구기관에서 실시
+* 기존 현장조사 담당자(근로감독관)가 전문 조사업체의 지원을 받아 실시할 수 있는 세부 실천 방안 수립 필요
+3.2.2 조사 모집단
+○ 저임금 근로자를 고용하고 있는 상용근로자 300인 미만 사업체의 사업주와 해당 사업체에 종사하고 있는 최저임금액 1.5배 이하 저임금 근로자를 대상으로 조사하는 것이 타당한지에 대해 재검토가 필요함(한국조사연구학회, 2020)
+- 조사대상인 저임금근로자에 대해 최저임금의 1.5배로 설정한 것은 2007년에 설정한 기준(2005년 최저임금 2,840원)이며 현재까지 어어져 옴
+- 최저임금이 2021년 현재 8,720원으로 2005년에 비해 3배 이상 상향된 현 상황에서 똑같이 사용하는 것이 적절한 지 검토 필요
+- 중위임금 대비 최저임금 수준을 보면 최근에는 최저임금이 중위임금의 약 2/3 수준으로 최저임금의 1.5배 = 중위임금으로서 조사대상이전체 근로자의 절반에 해당하는 상황임
+&lt;참고: 용어 정의&gt;
+• 최저임금(액)(minimum wage)
+- 근로자에 대하여 법적으로 보장된 임금의 최저수준
+• 중위임금(median wage)
+- 임금을 가장 낮은 수준부터 가장 높은 수준까지 정렬했을 때 50분위의 위치에 해당하는 임금수준. 즉, 임금분포 상에서 하위 임금자들과 상위 임금자들의 비율이 각각 50%가 되게 하는 임금수준
+3.2.3 표본추출틀
+○ 고용형태별 근로실태조사와 사업체노동실태현황을 활용한 2중 추출 방식은다소 복잡할 뿐만 아니라 시의성도 떨어짐(한국조사연구학회, 2021)
+- 조사대상 선별 시점에서 활용되는 고용형태별 근로실태조사 자료는 이전 연도의 자료가 활용되기 때문에 시의성이 떨어짐
+○(개선안)시의성 있고 표본 규모가 큰 사업체노동실태현황(214만개 표본보유, 매년 갱신)을 표본추출틀로 사용
+3.2.4 표본크기(목표)
+○ 상대표준오차를 적용하여 분석하거나 모집단 사업체수 비례 기준의 가중값을 부여할 경우 사업체 부문 조사의 적정 표본 크기는 3,500개로 파악됨(한국조사연구학회, 2021)
+○(개선안)사업체 3,500개; 근로자 10,000명
+3.2.5 층화
+○ 현행 실태조사에서 조사 대상이 되는 10개의 산업 분류는 2007년에 조사된고용형태별 근로실태조사 결과에 기반한 것이어서 15년 정도가 지난 현 시점에서 과연 그러한 조사 대상 산업분류가 여전히 유효한지 검토가 필요함(한국조사연구학회, 2020)
+○(개선안)종사자 규모는 기존과 동일하게 6개 범주로 유지하되, 업종은17개로 확대
+3.2.6 표본배분
+○ 현행 단순 비례배분 방식은 통계작성이나 추정에 있어 간편하다는 장점이 있으나, 크기가 작은 층에 표본이 작게 배분되어 층별 표본오차 관리가어렵다는 단점이 있음
+○(개선안)층별 통계작성이 용이한 제곱근 비례배분 방식의 표본배분
+3.2.7 가중치
+○ 현행 실태조사에서는 표본에 대해 가중치를 적용하지 않아 전체 모집단에 대한 추정이 불가능함
+○(개선안)표본배분표와 조사완료된 표본사업체의 분포의 차이가 발생하므로 산업대분류 및 사업체 규모의 분포를 반영하기 위해 가중치를 적용(한국조사연구학회, 2021)
+제3장 조사대상 선정기준의 적절성 검토를 위한 논의
+○'최저임금 적용효과에 관한 실태조사'에서는 조사대상을 저임금 근로자로 설정하고 있으며, 조사대상 저임금 근로자는 ‘최저임금액의 1.5배 이하의 임금 근로자’로 명시하고 있음
+○ 이러한 선정 기준은 조사가 시작된 2007년도의 임금분포(고용형태별 근로실태조사)에 근거하고 있으며, 당시의 기준으로는 이러한 조사대상 저임금근로자의 범위가 충분히 설득력이 있었으나, 상당 시간이 흐른 현재에도 이러한 기준이 합리적이고 타당한지에 대해서는 검토가 필요함
+○ 이번 장에서는 조사대상 선정기준의 적절성을 검토하고 조사대상 선정기준을 명확히 하는데 도움을 줄 수 있는 다양한 실증적 결과들을 살펴봄
+1. 저임금 근로자의 정의
+○ 저임금(low wage 또는 low pay)의 개념은 크게 ‘절대적’ 저임금과 ‘상대적’ 저임금으로 분류될 수 있으나, 통상적으로 저임금이라 함은 상대적 저임금을 의미함(&lt;|start|&gt;#@이름1#&lt;|end|&gt;, 2014;&lt;|start|&gt;#@이름2#&lt;|end|&gt;, 2011;&lt;|start|&gt;#@이름3#&lt;|end|&gt;, 2005)
+- 절대적 저임금은 ‘최소한의 일상생활을 위해 필요한 재화와 서비스를 구매할 수 있는 수준 이하의 임금’으로서 최저생계비, 빈곤선 등 특정 임금 수준 이하의 임금으로 측정되며, 나라마다 서로 그 수준이 달라 국가간 비교가 어려움
+- 다만, 절대적 저임금 근로자 비중의 국제비교를 위해 편의상 p10(하위 10분위 임금)지표가 활용됨
+- 상대적 저임금은 OECD 등 대부분의 국제기구에서 ‘중위임금(median wage)의 2/3 이하의 임금’으로 정의되며 국가간 비교 시 통상적인 저임금 근로자 선정기준으로 활용되고 있음
+- 저임금 근로자와 관련된 거의 모든 국내 연구들은 OECD의 상대적 저임금 개념을 활용하고 있음(&lt;|start|&gt;#@이름4#&lt;|end|&gt;, 2011;&lt;|start|&gt;#@이름5#&lt;|end|&gt;, 2014;&lt;|start|&gt;#@이름6#&lt;|end|&gt;, 2005; 현대경제연구원, 2014; 경기도가족여성연구원, 2016;&lt;|start|&gt;#@이름7#&lt;|end|&gt;, 2015;&lt;|start|&gt;#@이름8#&lt;|end|&gt;, 2018;&lt;|start|&gt;#@이름9#&lt;|end|&gt;, 2019;&lt;|start|&gt;#@이름10#&lt;|end|&gt;, 2011;&lt;|start|&gt;#@이름11#&lt;|end|&gt;, 2011 등)
+- OECD(OECD Data)에서는 임금 수준을 기준으로 저임금(low pay)근로자 비중과 고임금(high pay)근로자 비중으로 구분하여 국제비교 통계를 제공하고 있으며, 여기서 저임금은 중위임금의 2/3 이하, 고임금은 중위임금의 1.5배 이상의 임금으로 정의됨
+○'최저임금 적용효과에 관한 실태조사'에서의 저임금근로자는 최저임금의 1.5배 이하의 임금근로자로 정의되고 있어 통상적인 개념에서의 저임금근로자 개념과 다름
+- 동 조사에서의 저임금 근로자의 정의는 동 조사의 조사목적과 조사의 편의성을 고려한 측면이 큼
+2.</t>
+  </si>
+  <si>
+    <t>○ 사업실행 및 집행
+단체가 계획한 단위사업에 따른 사업실행 및 그에 따른 예산집행을 보조금 교부 이후부터 12월 31일까지 진행함. ○ 교육 및 워크숍 진행
+단체들의 사업 이해도 향상과 역량강화를 위해 총 4회 역량강화교육 및 2회 워크숍을 진행함. 2020년의 경우 코로나19로 대면회의가 어려워짐에 따라 워크숍과 모든 교육을 온라인으로 진행함. &lt;워크숍 및 교육 추진현황&gt;
 ○ 중간평가 및 2차 교부금 지급
-단체역량 및 운영과정을 중심으로 중간평가를 진행하고, 그 결과에 따라 2차 교부금 지급을 진행함. 2020년의 경우 코로나19로 인해 지원단체 선정에서부터 전반적인 사업추진 일정이 지연됨에 따라 중간평가 및 2차 교부도 다소 늦어짐. 코로나19로 인한 사업추진 가능성을 지켜보는 가운데 중간평가 시점에서 사업전체를 중도 포기하거나 2차 보조금 교부를 포기한 단체들도 다수 발생함. 
-○ 최종평가 및 정산
-전체 지원단체를 대상으로 사업평가와 회계평가를 진행하고 종합적으로 단체별 평가등급을 산출함. 또한, 전체 집행금액에 대한 평가를 진행하고 부적정 금액 및 이자 반환금액을 확정하여 정산을 진행함. 
-2. 평가개요
+단체역량 및 운영과정을 중심으로 중간평가를 진행하고, 그 결과에 따라 2차 교부금 지급을 진행함. 2020년의 경우 코로나19로 인해 지원단체 선정에서부터 전반적인 사업추진 일정이 지연됨에 따라 중간평가 및 2차 교부도 다소 늦어짐. 코로나19로 인한 사업추진 가능성을 지켜보는 가운데 중간평가 시점에서 사업전체를 중도 포기하거나 2차 보조금 교부를 포기한 단체들도 다수 발생함. ○ 최종평가 및 정산
+전체 지원단체를 대상으로 사업평가와 회계평가를 진행하고 종합적으로 단체별 평가등급을 산출함. 또한, 전체 집행금액에 대한 평가를 진행하고 부적정 금액 및 이자 반환금액을 확정하여 정산을 진행함. 2. 평가개요
 1)평가 추진개요
-○ 추진근거</t>
-  </si>
-  <si>
-    <t>[참고]단체별 종합평가 결과
-□ 1유형
-4. 회계 전문가 집행평가 검증
-◯ 2020년도 행정안전부 비영리민간단체 공익활동 지원사업 전체 단체 집행평가 내역에 대한 회계사 검증을 아래와 같이 실시함. 
-&lt;전문가 검증 개요&gt;
-◯ 집행평가 검증 결과 지적된 오류는 증빙서류 중 일부가 누락된 건이 대부분이었으며, 동일 집행 건에 대한 중복지급 문제도 발견됨. 
-◯ 검증 결과 문제가 제기된 단체에 대하여 소명‧보완과정 및 재평가 과정을 거쳐 지적된 건을 적법하게 수정‧처리함. 
-· 검증 완료 : ~2021년 2월 19일
-· 검증결과 반영 평가 수정 및 단체 보완, 재평가 완료 : ~2021년 2월 25일
-· 정산 반영 : ~2020년 2월 26월
-[제3장]
-결론
-1. 사업평가 시사점
-1)‘단체역량’ 항목 주요 시사점
-◯ 수요조사 및 사업개발노력</t>
-  </si>
-  <si>
-    <t>&lt;유형별 평가대상 단체 수&gt;
+○ 추진근거
+본 평가는 「비영리민간단체지원법 시행령」, 「2020년 비영리민간 단체 공익활동 지원사업 집행지침」에 근거하여 실시하였으며, 2020년 비영리민간단체 공익활동 지원사업에 참여한 단체가 제출한 최종보고서와 평가단의 현장평가 결과를 바탕으로 사업 측면에서 단체의 추진역량, 운영과정, 사업성과를, 회계 측면에서 사업비 집행의 적절성 등을 평가함. ○ 평가대상
+본 평가는 2020년 비영리민간단체 공익활동 지원사업에 선정된 223개 단체 중 코로나19 등의 이유로 사업포기 및 중도포기를 한 36개 단체를 제외한 187개 단체 사업에 대해 평가를 진행함. &lt;유형별 평가대상 단체 수&gt;
 ○ 평가내용
 본 평가는 단체들이 수행실적 및 사업성과 등에 대해 종합 작성한 최종보고서와 평가단에서 수행한 현장점검 결과를 바탕으로 수행함. 중간평가 시 사업평가 항목 중 단체역량과 운영과정 부문의 중간점검 및 집행실적 점검을 진행함으로써 성과 제고를 도모함. 최종평가는 사업평가와 회계평가로 진행하였으며, 사업평가의 경우 중간평가 시 진행된 단체역량, 운영과정 상의 평가를 단체들의 최종실적에 맞
-춰 재평가함과 동시에 사업성과 부분에 대한 집중평가를 평가지표에 의해 진행함. 
-회계평가는 전자증빙 사용률 등의 계량적인 회계평가 지표에 의해 평가를 진행함. 
-2)평가체계 및 항목
+춰 재평가함과 동시에 사업성과 부분에 대한 집중평가를 평가지표에 의해 진행함. 회계평가는 전자증빙 사용률 등의 계량적인 회계평가 지표에 의해 평가를 진행함. 2)평가체계 및 항목
 ○ 평가체계
-비영리 민간단체 지원사업 평가는 사업평가와 회계평가로 나뉘어 진행됨. 사업평가 항목은 단체역량, 운영과정, 성과 등 3개 항목, 총 13개 세부항목으로 구성되며, 회계평가 항목은 정산자료 구비상태 등 총 9개 항목으로 구성됨. 
-○ 사업평가 항목</t>
-  </si>
-  <si>
-    <t>&lt;사업평가 항목&gt;
+비영리 민간단체 지원사업 평가는 사업평가와 회계평가로 나뉘어 진행됨. 사업평가 항목은 단체역량, 운영과정, 성과 등 3개 항목, 총 13개 세부항목으로 구성되며, 회계평가 항목은 정산자료 구비상태 등 총 9개 항목으로 구성됨. ○ 사업평가 항목
+· 사업평가는 단체역량, 운영과정, 성과 총 3개 항목에 대한 평가로 진행되며, 단체역량에서는 사전 수요조사를 통해 사업개발을 위한 노력을 하였는가, 사업을 추진하기에 적합한 조직을 보유하고 있는가, 사업수행에 있어 기본이 되는 서류관리 등 행정관리가 제대로 진행되고 있는가를 평가함. · 운영과정에서는 효율적 사업수행을 위한 내·외부 협력체계를 잘 구축하고 있는가, 다양한 채널을 통해 사업홍보를 적극적으로 진행하고 있는가, 사업 대상자 확보를 위한 노력을 얼마나 기울이고 있는가, 사업이 회의를 통해 협의되고 공유된 형태로 추진되고 있는가를 평가함. · 마지막으로 성과에서는 본 사업이 계획한 목표를 달성하였는가, 사회적으로 얼마나 의미 있는 성과를 창출하였는가, 수혜자들이 만족할만한 수준의 사업을 진행하였는가를 종합적으로 평가함. &lt;사업평가 항목&gt;
 ○ 회계평가 항목
-· 회계평가는 사업비 사용의 적법성, 적정성 등을 평가하는 체계로 정산자료 구비상태, 사업비(보조금/자부담)집행률, 사업계획 변경의 적정성, 사업비(보조금/자부담)사용의 적법성, 전자증빙 사용률 등 총 9개 항목으로 평가함. 
-- NPAS 사업비 지연 등록 비율 20% 미만10
+· 회계평가는 사업비 사용의 적법성, 적정성 등을 평가하는 체계로 정산자료 구비상태, 사업비(보조금/자부담)집행률, 사업계획 변경의 적정성, 사업비(보조금/자부담)사용의 적법성, 전자증빙 사용률 등 총 9개 항목으로 평가함. - NPAS 사업비 지연 등록 비율 20% 미만10
 3)평가결과 산정
 ○ 평점부여
-· 사업평가 점수는 가·감점을 제외한 평가항목별로 우수, 보통, 미흡의 3단계로 평가함. 
-· 평가점수는 중간 및 최종평가에 걸쳐 총 2회 산출되었으며, 최종평가 시 중간평가 결과를 단체 최종실적에 맞게 업데이트하여 단체역량, 운영과정, 사업성과 부분의 평가점수를 확정지음. 
-○ 최종 평가점수 산출
-· 평가 시 사업평가, 회계평가를 각각 100점 만점 기준으로 점수를 부여하고, 종합적으로 사업평가 점수를 60점으로, 회계평가 점수를 40점으로 환산하여 단체별 최종 평가점수 및 등급을 산출함.</t>
-  </si>
-  <si>
-    <t>◯ 자체평가
-· 대다수의 단체들이 자체적으로 2020년도 사업수행에 대하여 우수하게 평가
-함. 다만, 코로나19로 인해 단위사업 일부를 수행하지 못하거나 계획했던 목표 달성을 이루지 못함에 따라 예년에 비해 자체평가에 있어 긍정적 평가가 근소하게 감소함. '19년에 95점 이상으로 ‘매우 우수’로 자체평가 한 단체들이'20년에는 90점 이상 수준으로 ‘우수’로 평가하는 수준의 하향세였음. 대부분의 단체들이 현실적으로 사업추진이 어려운 상황에서도 불구하고 사업추진을 위한 노력을 경주했다는 측면에서 자체적으로 긍정적인 평가를 한 것으로 판단됨. 
-· 자체평가의 경우 사업보고서 작성을 담당하는 사업 담당자 측면에서 긍정적으로 평가할 수밖에 없으므로 담당자 1인의 의견이 아닌 단체 이사회나 사업 위원회 차원에서 최종평가 시 평가해보고 이를 종합하여 자체평가 결과로 도출해내는 방식으로 체계화시킬 필요가 있음. 
-◯ 사회적 기여도</t>
+· 사업평가 점수는 가·감점을 제외한 평가항목별로 우수, 보통, 미흡의 3단계로 평가함. · 평가점수는 중간 및 최종평가에 걸쳐 총 2회 산출되었으며, 최종평가 시 중간평가 결과를 단체 최종실적에 맞게 업데이트하여 단체역량, 운영과정, 사업성과 부분의 평가점수를 확정지음. ○ 최종 평가점수 산출
+· 평가 시 사업평가, 회계평가를 각각 100점 만점 기준으로 점수를 부여하고, 종합적으로 사업평가 점수를 60점으로, 회계평가 점수를 40점으로 환산하여 단체별 최종 평가점수 및 등급을 산출함. · 최종 종합점수 90점 이상은 ‘우수’ 등급으로, 60점 이상 90점 미만은 ‘보통’ 등급으로, 60점 미만은 ‘미흡’ 등급으로 단체별 평가등급을 부여함. [제2장]
+평가결과
+1. 평가결과 종합
+1)종합평가 결과
+◯ 2020년도 행정안전부 비영리민간단체 공익활동 지원사업 종합평가 결과 사업평가 평균 80.34점, 회계평가 평균 92.16점, 종합 85.06점으로 집계되었음. ◯ 종합점수는 작년 대비 1점이 상승하여 2018년 이후부터 지속적으로 상승하는 경향을 보여주고 있음. ◯ 그러나, 사업평가의 경우 2017년부터 2019년까지 꾸준히 상승하다가 2020년 80.34점으로 작년대비 3.65점이 하락한 결과를 보여주었음. 이는 코로나19 팬데믹의 영향으로 대부분의 단체들이 사업내용이나 방식을 변경해야 했는데, 이로 인해 다수 단체가 일정 내 계획된 단위사업 모두를 수행하지 못함에 따라 성과 측면의 점수가 하락된 결과로 분석됨. ◯ 회계평가 점수는 평가항목 중 다른 항목에 비해 평균 점수가 낮아 항목간 평균 점수 편차가 심한 지표인 ‘지연일수 발생건수’를 ‘지연일수 발생비율’로 개선함에 따라 개선되었음. 또한, 집행지침에 대한 개별 컨설팅을 진행하고, 집행등록 관련 평가 프로세스를 보완‧강화함에 따라 회계평가 점수가 상승한 것으로 판단됨. &lt;연도별 종합평가 결과&gt;
+◯ 종합평가 결과 최고점은 96.19점(2유형 단체), 최저점은 58.40점(4유형 단체)으로 최고점과 최저점의 격차는 37.79점으로 나타남. ◯ 종합평가 결과 대다수의 단체가 70~90점대에 분포하고 있어 ‘보통’ 수준의 등급으로 평가되었으며, 90점 이상의 우수사업과 60점 미만의 미흡사업이 비교적 소수 분포하고 있음. &lt;2020년 종합평가 결과&gt;
+◯ 종합평가 결과 90점 이상인 우수등급 사업은 30개(16%), 90점 미만에서 60점 이상인 보통등급 사업은 156개(83%), 60점 미만인 미흡등급 사업은 1개(1%)인 것으로 집계됨. ◯ 종합평가 결과 가장 점수가 높은 상위 5개 단체는 2유형이 2개, 4유형이 2개, 6유형이 1개 단체로 분포되어 있으며, 이들 단체 모두 사업평가와 회계평가 점수가 90점 이상으로 매우 우수함. 종합 평가 점수는 1개 단체를 제외하고 모두 95점을 상회하였으며, 특히 회계평가 점수는 모두 95점 이상을 기록하였음. &lt;종합평가 결과 상위 5개 우수단체&gt;
+◯ 종합평가 결과 가장 점수가 낮은 미흡 5개 단체는 2유형이 1개, 4유형이 1개, 7유형이 3개로 분포되어 있으며, 이들 5개 단체 모두 사업평가에 있어 50점에서 60점대 점수를 받아 사업 운영성과가 미흡한 것으로 나타남. 2020년도에는 코로나19의 영향으로 해외 출입국이 불가능한 상황이 발생함에 따라 특히 7유형 국제교류 사업들이 미흡하게 추진된 측면이 있음. 사업평가 점수에 비해 회계 점수는 90점대에서 50점대까지 다양하게 분포함. &lt;종합평가 결과 하위 5개 미흡단체&gt;
+2)사업평가 결과
+◯ 사업평가 결과 평균점수는 80.34점으로 나타났으며, 최고점은 96.98점(2유형), 최저점은 57.58점(2유형)으로 최고점과 최저점의 격차는 39.4점으로 상당한 격차를 보임. ◯ 사업평가 결과 상당수의 단체들이 80점에서 90점 사이에 분포되어 있었으며, 그 다음으로 70점에서 80점 사이에 분포되어 있는 그룹이 차순위인 것으로 나타남. 대부분의 단체들이 코로나19로 인한 어려움에도 불구하고 다양한 노력을 통해 원활하게 사업을 추진함. &lt;2020년 사업평가 결과&gt;
+◯ 사업평가 결과 90점 이상인 우수 등급 사업은 22개(12%), 90점 미만에서 60점 이상인 보통 등급 사업은 161개(86%), 60점 미만인 미흡 등급 사업은 4개(2%)
+인 것으로 나타남. 평가 대상 중 대부분의(98%)사업이 보통 이상 등급으로 코로나19 팬데믹 영향에도 불구하고 비교적 원활하게 사업을 추진하였음을 보여줌. ◯ 사업평가 항목별 평균점수는 단체역량이 79.67점, 운영과정이 80.95점, 사업성과가 76.92점으로 100점 환산점수를 기준으로 했을 때 운영과정 측면의 단체 평균이 80.95점으로 가장 우수한 것으로 나타남. ◯ 항목별 평가등급 현황에서도 운영과정에서 우수등급을 받은 사업이 30개로 가장 많았으며, 사업성과에서 미흡등급을 받은 사업이 14개로 가장 많았음. 특히, 역량강화교육 수강 및 자체적인 역량 강화 자구책을 통해 코로나19 팬데믹 비상 상황에 비교적 잘 대처한 것으로 보임. 그러나, 외부 영향으로 인해 상당수의 사업에서 정상적인 추진이 어려워 사업 형태를 변경하거나 일부 단위사업을 취소할 수밖에 없었으며, 이로 인해 사업성과 창출 효과가 다소 미흡한 것으로 나타남. &lt;사업평가 세부영역별 평가결과&gt;
+◯ 사업평가 결과 가장 점수가 높은 상위 5개 우수단체는 2유형에 3개, 4유형에 1개, 6유형에 1개로 분포되어 있음. 5개 단체들 모두 90점 이상을 기록하였으며, 95점 이상을 기록한 단체는 1개였음. ◯ 상위 5개 단체 중 2유형의 1개 단체가 단체역량, 운영과정, 사업성과 측면에서 모두 우수 등급을 받음. 나머지 2유형 단체 1개와 4유형 단체 1개, 6유형 단체 1개는 단체역량과 운영과정 항목에서만 우수 등급으로 평가되었으며, 나머지 2유형 단체 1개는 사업성과 항목에서만 우수 등급으로 평가되었음. &lt;사업평가 결과 상위 5개 우수단체&gt;
+◯ 사업평가 결과 가장 점수가 낮은 하위 5개 미흡단체는 2유형에 2개, 5유형에 1개, 6유형에 2개 단체가 분포되어 있었음. 1개 단체를 제외하고 모두 60점 이하의 사업평가 점수를 기록하였음. ◯ 5개 미흡단체 모두 사업성과 영역에서 미흡하였으며, 그에 비해 단체역량 및 운영과정 항목은 보통 등급을 기록하였음. &lt;사업평가 결과 하위 5개 미흡단체&gt;
+3)회계평가 결과
+◯ 회계평가 결과 평균점수는 92.16점으로 나타났으며, 최고점은 100점(2유형_(재)사랑의장기기증운동본부 외 7개), 최저점은 52점으로 최고점과 최저점 간 48점의 상당한 격차를 보였음. ◯ 회계평가 결과 다수사업이 90점에서 100점 사이에 분포되어 있으며, 집행지침 관련 교육의 영향으로 사업평가 결과와 달리 소수 사업을 제외하고 모두 80점 이상에 분포되어 있는 것으로 나타남. &lt;2020년 회계평가 결과&gt;
+◯ 회계평가 결과 90점 이상인 우수등급 사업은 150개(80%), 90점 미만에서 60점
+이상인 보통등급 사업은 35개(19%), 60점 미만인 미흡등급 사업은 2개(1%)인 것으로 나타남. ◯ 회계평가 항목별 평균점수는 정산자료 구비 4.79, 보조금 집행률 3.66, 자부담 집행률 4.01, 계획변경 적법성 4.58, 보조금 집행 적법성 23.72, 자부담 집행 적법성 19.85, 전자증빙 사용비율 4.75, 집행등록 지연건수 7.90, 사업실적 대비 사업비 집행률 18.89점임. 100점 환산점수를 기준으로 했을 때, 자부담 집행 적법성 측면이 99점으로 가장 우수하며, 보조금 집행률이 73점으로 가장 미흡한 것으로 나타남. ◯ 사업 정산 시까지 보조금 및 자부담 집행에 대한 부적정건 보완 및 재평가, 이의신청 평가 등을 진행하여 보조금 및 자부담 집행 적정건수를 제고하였으며, 이에 따라 해당 항목이 우수하게 평가됨. 반면 코로나19 팬데믹의 영향으로 사업 진행이 원활하지 못했던 단체가 많아 보조금 집행률 점수가 가장 낮게 나타난 것으로 보임. ◯ 항목별 평가등급 현황을 살펴보면, 정산자료 구비, 계획변경 적법성이나 보조금 및 자부담 집행 적법성, 전자증빙 사용비율, 실적 대비 사업비 집행률에 있어서는 우수 등급을 받은 단체가 100개 이상으로 양호한 상황이었으나, 보조금 및 자부담 집행률, 집행등록 지연비율 등에서 미흡 등급을 받은 단체가 20개 이상으로 해당 영역에서 단체들의 실적이 다소 미흡한 것으로 나타남. 다만, ‘집행등록 지연건수’ 평가항목은 다른 평가항목들에 비해 평균점수 편차가 많이 발생하는 문제를 개선하기 위해 ‘집행등록 지연비율’로 지표를 개선함에 따라 회계평가 평균점수가 전년 대비 약 5점 가량 상승하였음. &lt;회계평가 항목별 평가결과&gt;
+◯ 회계평가 결과 가장 점수가 높은 상위 8개 우수단체는 2유형에 2개, 3유형에 3개, 4유형에 1개, 5유형에 2개로 집계됨. ◯ 8개 우수단체 모두 회계평가 전 영역에서 우수 등급을 받음. 회계평가 우수단체의 경우 정산자료 증빙에서부터 집행률, 계획변경 및 집행 적법성, 전자증빙, 실적 대비 사업비 집행에 있어서까지 회계 전 과정에서 우수하게 진행된 것으로 나타남. ◯ 회계평가 결과 가장 점수가 낮은 하위 2개 미흡단체는 4유형에 2개가 분포되어 있음. 이들 2개 미흡단체 모두 보조금 집행등록 평가에서 부적정 비율이 높아 보조금 사용 적법성 부분에서 모두 미흡으로 평가됨. ◯ 정산자료 구비 적절성의 경우 집행등록 평가에서 부적정 평가를 받은 단체들의 다수가 정산자료 구비 상태가 미흡한데에서 기인함에 따라 해당 지표에서 미흡등급을 받게 됨. ◯ 또한, 이들 단체들의 경우 집행 15일 내 등록 기준을 충족시키지 못하는 집행등록 건수가 많아서 집행등록 지연비율 항목에서 미흡 또는 보통으로 평가됨. &lt;회계평가 결과 하위 2개 미흡단체&gt;
+2. 사업유형별 평가결과
+1)유형별 평가결과 종합
+◯ 2020년도 행정안전부 비영리민간단체 공익활동 지원사업은 총 7개 유형으로 추진되었으며, 종합평가 결과는 다음과 같음. &lt;유형별 평가결과 종합&gt;
+※ 전체 평균값은 187개 단체 개별 데이터를 모수로 한 평균값임. (유형별 평균의 평균이 아님. )
+◯ 유형별 평가결과를 보면 7개 유형 모두 사업평가 보다 회계평가 점수가 높았음. ◯ 1유형 사회통합의 종합평가 점수가 88.45점으로 가장 높았고, 5유형 평화증진 및 국가안보의 종합점수가 82.26점으로 가장 낮았음. 종합평균의 최고점 유형과 최저점 유형 간의 점수 차는 6.19점으로 나타남. ◯ 유형별 평가결과를 평가 단위별로 살펴보면 1유형이 사업평가와 회계평가, 두 평가 단위에서 모두 가장 우수한 것으로 평가되었음. 반면, 5유형은 사업평가에서, 7유형은 회계평가에서 가장 미흡한 것으로 평가됨. ◯ 사업평가의 최고점 유형(1유형_84.54점)- 최저점 유형(2유형_78.38)간의 점수 차는 6.16점이며, 회계평가의 최고점 유형(1유형_94.31점)- 최저점 유형(7유형_86.95점)간의 점수 차는 7.36점으로 회계평가의 최고점 유형과 최저점 유형 간 점수 차가 사업평가의 최고점 유형과 최저점 유형 간 점수 차보다 약간 크게 나타남. 2)유형별 사업평가 결과
+◯ 사업평가의 항목별 평가결과를 사업유형에 따라 살펴보면 다음과 같음.</t>
+  </si>
+  <si>
+    <t>따라서 여성관리자패널조사는 제외한 나머지 유사통계 및 농림축산식품부의 귀농귀촌실태조사의 예산을 비교 검토하였다. - 2018 여성농업인 실태 조사 : 일반여성농업인 1,500가구, 귀농여성농업인 250가구, 다문화 여성 250가구, 총 2,000가구를 조사하였으며, 약 8천만원의 예산이 배정되었다. 조사비용은 건당 약 4만원이다. - 2021 농어업인등에 대한 복지실태조사 : 농어촌 4,000가구(가구 내적격 가구원)를 조사하였으며, 약 3억5천만원의 예산이 배정되었다. 조사비용은 건당 약 8만원이다. - 전국다문화가족 실태조사 : 전국 16,000가구(가구 내 적격 대상자)를 조사하였으며, 약 16억원의 예산이 배정되었다. 조사비용은 건당 약10만원이다. - 양성평등 실태조사: 전국 4,500가구를 조사하였으며, 약 4억 4천만원의 예산이 배정되었다. 조사비용은 건당 약 10만원이다. - 2020 귀농귀촌실태조사 : 전국 귀농귀촌 4,000가구(귀농 2,000가구및 귀촌 2,000가구)를 조사하며, 약 4억의 예산이 배정되었다. 조사비용은 가구 건당 약 10만원이다. - 2021 귀농귀촌실태조사 : 전국 귀농귀촌 6,000가구(귀농 3,000가구및 귀촌 3,000가구)를 조사하며, 약 5억의 예산이 배정되었다. 조사비용은 가구 건당 약 8만원이다. 2018년 여성농업인 실태조사의 경우 농촌지역 다문화여성 조사를 위해서조사자 외에 통역자를 동반하는 등 면접조사의 비용이 타 조사대비 높았음에도 불구하고, 다른 조사와 비교할 때 조사비용이 낮은 것을 알 수 있다. 또한조사 규모 역시 일반 가구를 대상으로 하는 타 조사의 절반에 미치지 못하는 것으로 나타난다. 따라서 조사의 정확성 및 대표성 확보를 위한 표본 수 확대와 적정 수준으로의 예산 증액이 필요한 것으로 여겨진다. 제 5 장 표본설계 개선방안
+제 1 절 표본설계 개선의 목적 및 방향
+여성농업인실태조사를 위한 표본설계의 개선을 위한 목적은 조사목표 및 통계산출을 위한 현행 표본설계의 적절성 평가 및 개선이다. 이를 위해 본연구에서는 여성농업인실태조사의 품질개선을 위해 조사모집단 변경을 반영하여 표본설계 개선안을 제안하고자 한다. 이러한 목적을 달성하기 위해 설정한 구체적인 목표는 다음과 같다. 첫째, 조사대상 변경 및 확대 검토
+둘째, 조사대상 변경을 반영한 표본크기 검토 및 제안
+셋째, 조사대상 변경에 따른 표본추출방법 개선방안
+넷째, 표본추출방법에 따른 모수 추정치 및 가중치 제시
+이를 위한 여성농업인실태조사 표본설계 개선방향은 다음과 같다. (1)조사 목적을 충실히 달성하기 위해서 합리적인 표본추출 및 표본배분원칙과 실사의 효율성을 높이도록 한다. (2)최신의 모집단 분석 결과와 2018년 조사데이터 분석 결과를 토대로표본배정을 위한 층화변수 등을 찾고, 다양한 표본배분 방법인 비례배분, 제곱근 비례배분, 네이만배분 등을 검토하고, 조사여건을 고려하여 최종 결정한다. (3)가중치 부여 과정을 포함해서 모수 추정식과 추정식의 오차계산 공식을 제시한다. 제 2 절 모집단 정의 및 분석
+1. 모집단과 조사항목
+1)모집단 및 표본추출틀 정의
+여성농업인실태조사의 목표모집단은 우리나라에 거주하는 여성농업인이나, 여성농업인통계가 존재하지 않으므로 농림어업총조사 가구명부를 표본추출틀로 하여, 농가 내 적격대상자를 조사하기로 한다. 즉 조사모집단은 2020년 농림어업총조사의 농가내 15세 이상 여성 중 농업에 종사하는 자9)이다. 표본추출틀은최신 모집단을 반영하기 위하여 2020년 농림어업총조사의 103만 5,193가구를대상으로 한다. 2)조사항목
+여성농업인실태조사의 조사항목은 인적사항, 기본사항, 가구현황, 경제·사회활동, 교육, 복지, 정책수요 및 향후계획의 7개 영역으로 구성된다. 인적사항및 기본사항 영역은 가구원별 현황, 혼인상태, 학력, 농업외 활동, 가구형태및 자녀 사항 등으로 구성되어 있으며, 가구현황 영역은 농가의 주요 생산품목, 토지면적, 연간농산물 판매금액, 자산, 농사일 담당비중, 가사 노동시간 등의항목으로 구성된다. 경제·사회활동 영역은 농업종사기간 및 이유, 평균 농업노동시간, 농업외소득, 여성농업인단체활동 등을 조사한다. 교육활동은 교육경험, 교육장소 및 일수, 희망교육 및 필요한 정책지원 등을 조사하며, 복지현황은 건강상태, 병원이용, 자녀 보육, 문화생활 등을 조사한다. 정책수요 및 향후계획은 농업활동 의향, 농촌거주 의향, 농업과 농촌에서의 애로사항, 여성의 지위, 여성농업인 정책에 대한 항목으로 구성되어 있다. 2.</t>
+  </si>
+  <si>
+    <t>이를 위해 ① 1기 계획의 문제와 과제를 2기 계획에서 보완해 나갈 내용과 과정 등을 제시. ② 1기 계획 실행기간 동안에 진행된 연차별 시행계획과의 연계성과 평가결과의 반영 등을 총괄하여 문제가 될 수 있는 부분을 개선해 나갈 수 있는 방향을 제시, ③ 이전 계획의 달성 정도도 평가. ④ 이전 지역사회복지계획의 후기 부분에 제시되어 있는 자체평가내용을 이번 계획에 어떻게 반영할 것인지를 검토함. 1.3 제2기 지역사회복지계획의 목적 및 목표
+1.3.1 제2기 지역사회복지계획의 목적
+○ 지방분권화 시대를 맞이하여 지역사회는 각종 사회복지정책이 집행되고 복지대상자를 대 상으로 사회복지서비스가 이루어지는 복지의 현장임. 따라서 지역주민과 복지대 상자들의 복지욕구를 정확히 파악하고 그 욕구를 바탕으로 지역실정에 적합하게 복지계획을 수립하고 시행함이 필요함. ○또한 지역에서 실시하고 있는 지역사회복지관련 서비스 실태를 파악하고 공급할 수 있는 복지자원의 활용 가능성을 확보하고 지역발전을 위한 각종 방안을 마련하여 복지정책 및 자원의 우선순위를 결정하는 복지계획 수립을 통해 지역주민의 복지증진이 가능해질 것임. ○ 따라서 용산구 제2기 지역사회복지계획 수립은 용산구의 복지수요와 현황을 진단하여 지역사회의 참여를 통한 지역실정에 맞는 복지계획과 향후 분야별 추진계획을 마련하여 지역사회복지 증진을 강화하고자 함. 1.3.2 제2기 지역사회복지계획의 목표
+○용산구 지역주망들의 복자욕구를 파악하고. 용산구의 복지자원과 복지정책을 분석하여. 보 건복지부의 복지정책과 서울시의 시정방향 그리고 지역적 특성을 고려한 용산구의 사회복지정책 방향을 구체적으로 실천할 수 있는 계획을 수립함. ○ 본 계획을 위해 용산구 관내의 지역복지자원의 유형과 규모, 내용 활동, 용산구의 사회복지 정책 및 서비스 등을 광범위하게 조사한 내용과 용산구 지역주민들의 지역복지에 대한 인 식과 복지서비스에 대한 만족도 및 문제점, 복지욕구 등을 설문조사를 통해 체계적으로 분 석한 자료를 활용함. 이를 기반으로 하여 용산구의 사회복지 비전과 방향을 제시하고, 중점 사업과 연차별 추진계획, 부문별 사업계획을 포함하는 용산구 지역사회복지계획을 수립함. 14 제2기 지역사회복지계픽의 성격
+• 지역사회중심의 사회복지제도화 
+지역사회복지계획은 각 지역의 특성이나 주민의 복지욕구, 사회자원의 과다. 정책현황 등에 대하여 조사를 실시함. 이 조사에서 드러나 문제를 해결하기 위해 주민 참여에 기반을 둔 민· 관 네트워크를 통하여 앞으로의 목표를 설정하고 이를 실현하는 데에 필요한 사회자원을 조 달하여 적정하게 배분하는 것에 대한 구체적인 실시를 약속하는 것임. 이러한 계획을 실현하 는 과정에서 지역사회에 필요한 사회복지가 제도적 형태로 구체화될 수 있음. • 지역사회복지서비스의 수급조정과 안정적 공급 
+지방자치제 하에서 지방정부는 각 지역사회에 있어서 복지서비스의 수급조정과 안정적 공급 을 위한 방안을 모색해야 하는데, 이것은 지역복지계획을 수립·실천해 나감으로써 해결될 수 있음. 지역사회복지계획에서는 일정한 목표를 정하고 그것을 달성하기 위한 방법이나 수단을 검토하게 됨. 지역사회목지계획을 통해 지역의 복지문제나 과제를 해결하는 데에 필요한 인적·물적 자원을 조달하여 적절히 분배하고 서비스의 수요와 공급의 균형을 조절함으로써 사회 복지 대상자에게 안정적·진송직으로 서비스를 공급할 수 있음. • 지역사회복지서비스 공급주체의 다원화
+지역사회가 지닌 복지욕구와 문제는 공공부문만으로는 해결하기 어려우며 다양한 민간단체들 이 참여해야 함. 지역복지계획은 중앙 및 지방 정부뿐만 아니라 지역사회 내의 다양한 민간 단체들을 끌어들여서 복지서비스의 공급에 참여하도록 촉구하게 됨. 이 계획에서는 기존의 사 회복지기관·시설이나 사회복지단체뿐만 아니라 자원봉사단체, 시민단체, 전문가단체 등도 복 지서비스의 공급주체로 설정됨. • 사회자원의 조달과 적정배분 
+지역사회복지계획을 수립하는 과정에서 보건·의료·복지·주택·고용 등에 관련된 공공 및 민간기관과 공동모금이나 기부금 등의 물적 자원과, 사회복지시설 종사자와 일반주민 등의 인적 자원을 개발·조달하는 방안이 제시되고 이것을 효율적으로 배분하기 위한 노력이 이루어짐. 1.5 제2기 지역사회복지계픽의 수립의 과정
+○ 사회복지사업법 제15조의3에 의거 제2기 지역사회복지계획（2011~2014년)을 수립하여 지역의 복지 비전과 실천계획을 제시하고, 지역차원의 사회복자공급의 통합, 참여, 협력을 촉진함으로써 지역사회복지 증진의 책임성을 강화하고자 지자체, 지역사회 복지협의체, 외부 학술용역기관을 중심으로 지역주민의 의견 수령 절차를 거쳐 다음과 같이 추진함. ○ 지역사회복지계획 추진 과정은 다음과 같음
+○ 2010년 4월 지역사회복지협의체, 지자체, 외부 학술용역기관을 계획 수립 실행 주체로 하 는 2011년에서 2014년까지 4개년 중기 지역사회복지계획 수립을 위한 기본 설계 및 지역 사회복지계획수립 TF를 구성함. ○ 2010년 5〜7월, 학술용역기관을 통해 사회복지 욕구조사 및 자원조사를 실시함. 지역주민 조사를 위한 설문 문항 선정 및 대상자 설문조사활동에는 지역 사회복지기관들이 참여하였으며 실무부서의 의견이 반영되었음. 서비스제공자조사, 주요정보제공자 조사의 일환으로 지역사회복지계획수립 TF팀 회의, 공공사업부서 실무자가 참여한 지역사회복지협의체 실무분과 자문회의가 있었음. ○ 용산구민의 복지욕구를 다각적으로 분석하기 위해 조사대상 집단을 지역구민, 노인, 저소득주민, 여성(영유아포함), 아동, 청소년, 장애인, 다문화 가정, 여론주도층, 실무자 집단으로 구분하였으며 지역사회복지 욕구조사를 심도 있게 실시함. ○ 2010. 10월에는 각 계층별 지역사회복지계획안 마련을 위해 용산구청, 지역사회복지협의 체, 학술연구용역팀, 보건소 및 동 주민 센터의 관련 공무원과 사회복지기관(시설)실무종사자를 중심으로 지자체의 의견 수령 및 검토과정이 있었음. ○ 2010. 11월에는 지역사회복지계획안에 대한 지역주민 의견 수렴과 지역사회복지대표협의체의 심의를 거쳐 제2기 용산구 지역사회복지계획이 확정됨. ○ 2010. 11월에는 지역사회복지계획의 최종보고는 서울시에 보고하고, 서울시의 권고·조정 사항을 반영하여 하반기에 최종계획이 확정됨. 2. 용산구 지역 및 복지자원 기본현황
+2.1 용산구 연혁
+□ 용산이라는 이름은 인왕산 줄기가 만리재길을 거쳐 청파동으로 이어지면서 한강으로 뻗어 내린 모습이 용의 생김새와 비슷하다 하여 붙여졌다는 설과, 백제 기루왕 21년(A. D 97)4월에 한강에 두 마리 용이 나타났다는 증보문헌비고의 기록에서 유래되었다고 함. □ 용산의 지명은 고려 숙종 6년(1101)남경 후보지의 하나로 거론되기도 하였고 충렬왕 10년(1284)에 는 과주의 용산처를 승격하여 부원현으로 하였다는 기록이 있어 이미 고려시대 이전에 용산은 한 고을명으로 존재하였음. □ 용산구는 1896년 4월 한성부 용산방으로 시작하여 1910년 10월 조선총독부에 의해 한성부가 경성부로 개창되면서 경기도에 편입됨. 1911년 4월 경성부내에 5부 8면제를 실시하 면서 용산방이 용산면이 되었음. □ 경성부의 인구가 1OO만명에 이르고 주거지역이 급속히 팽창하연서 1943년 6월 ‘구제 ’를 실시, 행정기관으로 용산구역소를 설치함. 1945년 10월 용산구역소의 명칭이 용산구로 개칭되고 1946년 서울특별시 용산구가 되었음. □ 그 후 경제발전과 인구변동 등으로 인해 여러 차례 관할 구역의 조정을 거치다가 1995년 7월 1일 민선 제1기 출범을 계기로 본격적인 지방자치시대로 접어들면서 오늘에 이르고 있음. 2.2 지역 일반현왕
+2.2.1 지리적 현황
+□ 서울의 중심부에 위치한 용산은 경제 및 교통, 문화의 중심지로서 효창공원, 용산가족공원, 전쟁기념관, 한강시민공원 등 도심공원이 많아 시민이 쾌적한 휴식을 즐길 수 있는 공간을 제공하고 있으며 연간 약 140만명이 방문하는 이태원 관광특구를 비롯하여 많은 외국 공 관서와 문화원, 용산전자상가, 미8군 등이 있어 외국인 거주자 및 출입자가 많은 지역임. □ 위치적으로 서울 중심에 있으면서도 지금까지 철도부지와 미군부대와 같은 걸림돌 등으로 낙후 이미지가 강했던 용산은 철도차량기지 일대 초고층 서울 랜드마크를 중심으로 하는 국제업무지구단지와 미군부대 이전에 따른 270만㎡의 대규모 생태공원 조성, 여기에 이 모든 공 간을 기본적으로 지하로 연결하는 통합입체공간인 용산링크 계획으로 가장 주목받고 있는 도시로 부각되고 있음. 2）지형 및 지질
+□ 용산의 지형은 남산이 위치한 북동쪽이 높고 남서쪽은 저평안 구릉지를 이루고 있음. 전체 적으로 보면 남산일대가 100m 내외의 산지이고 대부분 50m 이하의 낮은 평지이다. 남산은 화강 암으로 이루어진 잔구성 산지이며 그 서쪽 저지대를 따라 욱천이 남류함. □ 용산구 지질은 대부분이 선캄브리아대의 경기편마암복합체로 되어 있으며, 북동부 일부지 역에는 쥐라기 대보화강암이 분포함. 그리고 남쪽 한강 연안에는 제4기 충적층이 동서로 길게 분포하고 있음. 3）교통
+□ 한강과 연결되는 서울의 관문인 용산은 조선시대에 조운선이 포구로 몰려들어 경강상인의 본거지였고 일제시대에는 용산을 기점으로 하거나 통과하는 철도가 많이 부설되고 각종 철도관계시설이 집중되면서 우리나라 철도망의 심장부 역할을 하였음. □ 용산은 국철 및 지하철 4·6호선과 한강의 6개 다리（한남·반포·동작·원효·한강대교, 한강철교）가 위치하는 지리적 이점으로 타도심과 강남 접근이 매우 용이하며, 경의선(용산~문산）, 중앙선（용산~용문)이 산설되어, 파주시를 비롯한 경기 북서부, 양평군을 포함하는 경기 서부 지역의 접근이 편리하게 되었음. □ 향후 송파신도시와 용산국제업무지구를 잇는 도시형 자기부상 방식의 급행철도가 건설될 경우 용산과 강남권의 이동시간이 불과 20~30분 이내로 단축될 것으로 예상하고 있음. 이와 더불어 현재 추진중인 신공항선(인천국제공항철도), 신분당선(분당~강남)이 완공되게 되면 용산은 명실공히 최고의 교통인프라를 갖춘 첨단 국제도시로서의 면모를 갖추게 될 것임. □ 국제업무지구단지 내의 국제여객·물류 터미널 계획은 용산뿐만 아니라 서울, 나아가 대한 민국 전체의 세계경제에 대한 접근성을 보다 용이하게 해줄 것이며, 현재 추진중인 경부선 복개안(용산역- 서울역), 경원선 지하화(용산역- 서빙고역）사업이 현실화 될 경우 지금까지의 철도시설물로 인한 지역간 단절과 교통대란이 대폭 해소될 것으로 예상됨. 2.2.2 전체 인구 및 복지대상별 인구 현황
+1）전체 인구 현황
+□ 2009년 12월 31일 기준 용산구 인구는 107,456세대에 238,708명임.</t>
+  </si>
+  <si>
+    <t>그러나 좀 더 국내의 대표성을 가지기 위해서는 참여기관을 수도권 이외의 지역으로 확대할 필요가 있다. - 참여의료기관의 특성 : KONIS를 기준으로 병원의 규모를 나누어 본다면 900병상이상이 3개 기관, 700-900병상 13개 기관, 400-700병상 8개기관, 400개 미만 기관은 8개 기관이다. 이중 KONIS에 참여하지 않는 병원 1개기관 뿐이며 모든 병원이 문제없이 surveillance monitoring이 가능하다. 연구의 목표를 달성하기 위해서는 다양한 규모와 역할의 병원이 참여하는 것이 필요하다. 병상 수를 볼 때 병상규모 별 모집은 큰 문제 없다. 그러나 역할에 있어 급성기 치료 역할을 하는 종합병원이 대부분이다. 지역사회감염의 중요한역할을 담당하는 특수병원의 참여가 거의 없어 이를 보완할 필요가 있다. 2017년도 구성에서는 요양병원1개 기관, 화상병원 1개기관이 참여했다. 참여 중환자실의 경우 대부분은 종합중환자실이었고, 특성화되어 있는 기관의 경우 외과계중환자실 12개 기관과 내과계중환자실 5개기관으로 대부분이 외과계중환자실 이었다. 2개 기관을 제외한 참여기관에서 자체적으로 미생물 검사실 운용을 하고 있어 요로감염 진단에 문제는 없었다. 요로감염 예방증진사업 기관 모집 안내문 
+안녕하십니까? 요로감염 예방증진사업 연구를 담당하는 연구책임자 한림대학교 강남성심병원 감염내과&lt;|start|&gt;#@이름1#&lt;|end|&gt;입니다. 요로감염 예방증진사업(질병관리본부 발주정책용역과제, 3년연속과제)은 대한의료관련감염학회에서 주관하고 한림대학교에서 실무를 맡아 대학병원과 중소병원의 의료관련 요로감염 예방을 위해 병원별로 요로감염 Bundle을 체계적으로 적용하여 효과를 분석하는 연구 사업으로 아래와 같이 참여 가능한 중소병원을 모집하고자 하오니 연구 취지에 공감하시는 중소병원 감염관리 실장님 또는 실무 담당자 분들께 적극적인 동참을 요청 드리며, 동참하여 주시면 요로감염 중재연구 사무국에서 개별병원의 요로감염 예방 활동에 충분한 지원이 되도록 노력하겠습니다. - 모집 안내 - 
+● 사업기간 : 2017년 6월 ~ 2019년 12월
+● 참여대상 : 300병상 이상의 중소병원 
+1)입원 환자를 대상으로 요로감염감시가 가능한 기관
+2)전임 감염관리간호사가 있는 기관
+● 신청기한 : 선착순 목표 기관수 도달 시까지
+● 신청방법 : 신청서를 작성하여 이메일로 접수 신청서 접수 시 파일명[신청일/병원이름](예 - 20170501 강남성심병원)으로 저장
+● 신청 및 문의 : E- mail iccon@iccon. or.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -254,15 +590,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -308,25 +637,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -364,7 +685,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -398,7 +719,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -433,10 +753,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -609,17 +928,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
-  <cols>
-    <col min="1" max="1" width="71.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -637,7 +951,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.76778459548950195</v>
+        <v>0.7085676193237305</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -648,7 +962,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.70565569400787354</v>
+        <v>0.5246601700782776</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -659,7 +973,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.69179123640060425</v>
+        <v>0.4905118048191071</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -670,10 +984,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.70294314622879028</v>
+        <v>0.718936026096344</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -681,10 +995,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.66151082515716553</v>
+        <v>0.6314802169799805</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -692,10 +1006,10 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>0.6165425181388855</v>
+        <v>0.5269343852996826</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -703,7 +1017,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>0.65324258804321289</v>
+        <v>0.6816848516464233</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -714,10 +1028,10 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0.63840430974960327</v>
+        <v>0.5292262434959412</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -725,10 +1039,10 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>0.60204291343688965</v>
+        <v>0.507931649684906</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -736,10 +1050,10 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>0.78874689340591431</v>
+        <v>0.7197926044464111</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -747,7 +1061,7 @@
         <v>6</v>
       </c>
       <c r="B12">
-        <v>0.73111337423324585</v>
+        <v>0.6418085098266602</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
@@ -758,10 +1072,10 @@
         <v>6</v>
       </c>
       <c r="B13">
-        <v>0.70228052139282227</v>
+        <v>0.6215807795524597</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -769,10 +1083,10 @@
         <v>7</v>
       </c>
       <c r="B14">
-        <v>0.71415603160858154</v>
+        <v>0.6775275468826294</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -780,10 +1094,10 @@
         <v>7</v>
       </c>
       <c r="B15">
-        <v>0.69139546155929565</v>
+        <v>0.6648162603378296</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -791,10 +1105,10 @@
         <v>7</v>
       </c>
       <c r="B16">
-        <v>0.67530035972595215</v>
+        <v>0.6117748022079468</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -802,10 +1116,10 @@
         <v>8</v>
       </c>
       <c r="B17">
-        <v>0.6359637975692749</v>
+        <v>0.5578191876411438</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -813,10 +1127,10 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <v>0.60413646697998047</v>
+        <v>0.5418356657028198</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -824,10 +1138,10 @@
         <v>8</v>
       </c>
       <c r="B19">
-        <v>0.60079479217529297</v>
+        <v>0.4851812720298767</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -835,10 +1149,10 @@
         <v>9</v>
       </c>
       <c r="B20">
-        <v>0.61809039115905762</v>
+        <v>0.5105457305908203</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -846,10 +1160,10 @@
         <v>9</v>
       </c>
       <c r="B21">
-        <v>0.60788595676422119</v>
+        <v>0.4931620955467224</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -857,10 +1171,10 @@
         <v>9</v>
       </c>
       <c r="B22">
-        <v>0.59058511257171631</v>
+        <v>0.4929372668266296</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -868,10 +1182,10 @@
         <v>10</v>
       </c>
       <c r="B23">
-        <v>0.51283884048461914</v>
+        <v>0.4714450240135193</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -879,10 +1193,10 @@
         <v>10</v>
       </c>
       <c r="B24">
-        <v>0.51194959878921509</v>
+        <v>0.3834758996963501</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -890,10 +1204,10 @@
         <v>10</v>
       </c>
       <c r="B25">
-        <v>0.50175690650939941</v>
+        <v>0.3618778586387634</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -901,10 +1215,10 @@
         <v>11</v>
       </c>
       <c r="B26">
-        <v>0.61505985260009766</v>
+        <v>0.4469998478889465</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -912,10 +1226,10 @@
         <v>11</v>
       </c>
       <c r="B27">
-        <v>0.58436459302902222</v>
+        <v>0.4413443803787231</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -923,10 +1237,10 @@
         <v>11</v>
       </c>
       <c r="B28">
-        <v>0.55696970224380493</v>
+        <v>0.4388315677642822</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -934,10 +1248,10 @@
         <v>12</v>
       </c>
       <c r="B29">
-        <v>0.61391103267669678</v>
+        <v>0.4564327597618103</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -945,10 +1259,10 @@
         <v>12</v>
       </c>
       <c r="B30">
-        <v>0.53353023529052734</v>
+        <v>0.4551244974136353</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -956,14 +1270,13 @@
         <v>12</v>
       </c>
       <c r="B31">
-        <v>0.50986087322235107</v>
+        <v>0.4027367234230042</v>
       </c>
       <c r="C31" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>